<commit_message>
Deploying to gh-pages from @ xkre/malaysia-inflation-calc@a4e4d37eb556be714f41a555a7133a9020860de8 🚀
</commit_message>
<xml_diff>
--- a/data/CpiDataset.xlsx
+++ b/data/CpiDataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Malaysia" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Sarawak" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Copy to Json" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="2021-2022" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Big Mac Index" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6862" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6866" uniqueCount="83">
   <si>
     <t xml:space="preserve">Period type</t>
   </si>
@@ -189,6 +190,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tempoh </t>
     </r>
@@ -198,6 +200,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Period</t>
     </r>
@@ -209,6 +212,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Jumlah  </t>
     </r>
@@ -218,6 +222,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Total</t>
     </r>
@@ -229,6 +234,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Makanan &amp; Minuman Bukan Alkohol       </t>
     </r>
@@ -238,6 +244,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Food &amp; Non-Alcoholic Beverages  </t>
     </r>
@@ -249,6 +256,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Minuman Alkohol &amp; Tembakau      </t>
     </r>
@@ -258,6 +266,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Alcoholic Beverages &amp; Tobacco  </t>
     </r>
@@ -269,6 +278,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pakaian &amp; Kasut     </t>
     </r>
@@ -278,6 +288,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Clothing &amp; Footwear       </t>
     </r>
@@ -289,6 +300,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Perumahan, Air, Elektrik, Gas &amp; Bahan Api Lain  </t>
     </r>
@@ -298,6 +310,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Housing, Water, Electricity, Gas &amp; Other Fuels</t>
     </r>
@@ -309,6 +322,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hiasan, Perkakasan &amp; Penyeleng-garaan Isi Rumah   </t>
     </r>
@@ -318,6 +332,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Furnishings, Household Equipment &amp; Routine Household Maintenance</t>
     </r>
@@ -329,6 +344,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Kesihatan </t>
     </r>
@@ -338,6 +354,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Health   </t>
     </r>
@@ -349,6 +366,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pengang-kutan  </t>
     </r>
@@ -358,6 +376,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Transport   </t>
     </r>
@@ -369,6 +388,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Komunikasi</t>
     </r>
@@ -378,6 +398,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -387,6 +408,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Communication               </t>
     </r>
@@ -398,6 +420,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Perkhidmatan Rekreasi &amp; Kebudayaan       </t>
     </r>
@@ -407,6 +430,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Recreation Services &amp; Culture</t>
     </r>
@@ -418,6 +442,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pendidikan </t>
     </r>
@@ -427,6 +452,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Education        </t>
     </r>
@@ -438,6 +464,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Restoran &amp; Hotel </t>
     </r>
@@ -447,6 +474,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Restaurants &amp; Hotels  </t>
     </r>
@@ -458,6 +486,7 @@
         <sz val="10"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pelbagai Barangan &amp; Perkhidmatan </t>
     </r>
@@ -467,6 +496,7 @@
         <sz val="9"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Miscellaneous Goods &amp; Services     </t>
     </r>
@@ -513,18 +543,28 @@
   <si>
     <t xml:space="preserve">AVERAGE</t>
   </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -568,6 +608,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="9"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
@@ -576,32 +630,16 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -882,60 +920,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="73" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -6075,7 +6113,7 @@
       <c r="D283" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E283" s="0" t="n">
+      <c r="E283" s="1" t="n">
         <v>124.2875</v>
       </c>
     </row>
@@ -6092,7 +6130,7 @@
       <c r="D284" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E284" s="0" t="n">
+      <c r="E284" s="1" t="n">
         <v>139.2</v>
       </c>
     </row>
@@ -6109,7 +6147,6 @@
       <c r="D285" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E285" s="0"/>
     </row>
     <row r="286" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
@@ -6124,7 +6161,7 @@
       <c r="D286" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E286" s="0" t="n">
+      <c r="E286" s="1" t="n">
         <v>93.1625</v>
       </c>
     </row>
@@ -6141,7 +6178,7 @@
       <c r="D287" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E287" s="0" t="n">
+      <c r="E287" s="1" t="n">
         <v>128.775</v>
       </c>
     </row>
@@ -6158,7 +6195,7 @@
       <c r="D288" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E288" s="0" t="n">
+      <c r="E288" s="1" t="n">
         <v>122.1125</v>
       </c>
     </row>
@@ -6175,7 +6212,7 @@
       <c r="D289" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E289" s="0" t="n">
+      <c r="E289" s="1" t="n">
         <v>125.2125</v>
       </c>
     </row>
@@ -6192,7 +6229,7 @@
       <c r="D290" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E290" s="0" t="n">
+      <c r="E290" s="1" t="n">
         <v>114.75</v>
       </c>
     </row>
@@ -6209,7 +6246,7 @@
       <c r="D291" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E291" s="0" t="n">
+      <c r="E291" s="1" t="n">
         <v>97.5</v>
       </c>
     </row>
@@ -6226,7 +6263,7 @@
       <c r="D292" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E292" s="0" t="n">
+      <c r="E292" s="1" t="n">
         <v>114.9</v>
       </c>
     </row>
@@ -6243,7 +6280,7 @@
       <c r="D293" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E293" s="0" t="n">
+      <c r="E293" s="1" t="n">
         <v>122.2125</v>
       </c>
     </row>
@@ -6260,7 +6297,7 @@
       <c r="D294" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E294" s="0" t="n">
+      <c r="E294" s="1" t="n">
         <v>137.95</v>
       </c>
     </row>
@@ -6277,7 +6314,7 @@
       <c r="D295" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E295" s="0" t="n">
+      <c r="E295" s="1" t="n">
         <v>118.45</v>
       </c>
     </row>
@@ -36316,7 +36353,7 @@
       <c r="E283" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F283" s="0" t="n">
+      <c r="F283" s="1" t="n">
         <v>124.2875</v>
       </c>
       <c r="G283" s="1" t="s">
@@ -36330,7 +36367,7 @@
       <c r="E284" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F284" s="0" t="n">
+      <c r="F284" s="1" t="n">
         <v>139.2</v>
       </c>
       <c r="G284" s="1" t="s">
@@ -36344,7 +36381,6 @@
       <c r="E285" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F285" s="0"/>
       <c r="G285" s="1" t="s">
         <v>38</v>
       </c>
@@ -36356,7 +36392,7 @@
       <c r="E286" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F286" s="0" t="n">
+      <c r="F286" s="1" t="n">
         <v>93.1625</v>
       </c>
       <c r="G286" s="1" t="s">
@@ -36370,7 +36406,7 @@
       <c r="E287" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F287" s="0" t="n">
+      <c r="F287" s="1" t="n">
         <v>128.775</v>
       </c>
       <c r="G287" s="1" t="s">
@@ -36384,7 +36420,7 @@
       <c r="E288" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F288" s="0" t="n">
+      <c r="F288" s="1" t="n">
         <v>122.1125</v>
       </c>
       <c r="G288" s="1" t="s">
@@ -36398,7 +36434,7 @@
       <c r="E289" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F289" s="0" t="n">
+      <c r="F289" s="1" t="n">
         <v>125.2125</v>
       </c>
       <c r="G289" s="1" t="s">
@@ -36412,7 +36448,7 @@
       <c r="E290" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F290" s="0" t="n">
+      <c r="F290" s="1" t="n">
         <v>114.75</v>
       </c>
       <c r="G290" s="1" t="s">
@@ -36426,7 +36462,7 @@
       <c r="E291" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F291" s="0" t="n">
+      <c r="F291" s="1" t="n">
         <v>97.5</v>
       </c>
       <c r="G291" s="1" t="s">
@@ -36440,7 +36476,7 @@
       <c r="E292" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F292" s="0" t="n">
+      <c r="F292" s="1" t="n">
         <v>114.9</v>
       </c>
       <c r="G292" s="1" t="s">
@@ -36454,7 +36490,7 @@
       <c r="E293" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F293" s="0" t="n">
+      <c r="F293" s="1" t="n">
         <v>122.2125</v>
       </c>
       <c r="G293" s="1" t="s">
@@ -36468,7 +36504,7 @@
       <c r="E294" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F294" s="0" t="n">
+      <c r="F294" s="1" t="n">
         <v>137.95</v>
       </c>
       <c r="G294" s="1" t="s">
@@ -36482,7 +36518,7 @@
       <c r="E295" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F295" s="0" t="n">
+      <c r="F295" s="1" t="n">
         <v>118.45</v>
       </c>
       <c r="G295" s="1" t="s">
@@ -36510,1382 +36546,1368 @@
   </sheetPr>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="n">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="n">
         <v>117</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="6" t="n">
         <v>125.1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="6" t="n">
         <v>98.2</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="6" t="n">
         <v>119.5</v>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="6" t="n">
         <v>114.4</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="6" t="n">
         <v>120.9</v>
       </c>
-      <c r="J2" s="8" t="n">
+      <c r="J2" s="6" t="n">
         <v>113.5</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="6" t="n">
         <v>97.7</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="L2" s="6" t="n">
         <v>111.5</v>
       </c>
-      <c r="M2" s="8" t="n">
+      <c r="M2" s="6" t="n">
         <v>116.7</v>
       </c>
-      <c r="N2" s="8" t="n">
+      <c r="N2" s="6" t="n">
         <v>128.2</v>
       </c>
-      <c r="O2" s="8" t="n">
+      <c r="O2" s="6" t="n">
         <v>114.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="4" t="n">
         <v>2018</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="n">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="n">
         <v>118</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="6" t="n">
         <v>127.4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="6" t="n">
         <v>96.2</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="6" t="n">
         <v>122.4</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="6" t="n">
         <v>114.8</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="6" t="n">
         <v>121.9</v>
       </c>
-      <c r="J3" s="8" t="n">
+      <c r="J3" s="6" t="n">
         <v>112.6</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="6" t="n">
         <v>96</v>
       </c>
-      <c r="L3" s="8" t="n">
+      <c r="L3" s="6" t="n">
         <v>111</v>
       </c>
-      <c r="M3" s="8" t="n">
+      <c r="M3" s="6" t="n">
         <v>118</v>
       </c>
-      <c r="N3" s="8" t="n">
+      <c r="N3" s="6" t="n">
         <v>130.2</v>
       </c>
-      <c r="O3" s="8" t="n">
+      <c r="O3" s="6" t="n">
         <v>112.6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="4" t="n">
         <v>2019</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="n">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="n">
         <v>119.3</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="6" t="n">
         <v>130.1</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="6" t="n">
         <v>94.3</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="G4" s="6" t="n">
         <v>125</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="6" t="n">
         <v>116.4</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="I4" s="6" t="n">
         <v>122.7</v>
       </c>
-      <c r="J4" s="8" t="n">
+      <c r="J4" s="6" t="n">
         <v>109.1</v>
       </c>
-      <c r="K4" s="8" t="n">
+      <c r="K4" s="6" t="n">
         <v>96.4</v>
       </c>
-      <c r="L4" s="8" t="n">
+      <c r="L4" s="6" t="n">
         <v>111.8</v>
       </c>
-      <c r="M4" s="8" t="n">
+      <c r="M4" s="6" t="n">
         <v>119.7</v>
       </c>
-      <c r="N4" s="8" t="n">
+      <c r="N4" s="6" t="n">
         <v>131.8</v>
       </c>
-      <c r="O4" s="8" t="n">
+      <c r="O4" s="6" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="4" t="n">
         <v>2020</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="n">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="n">
         <v>120.6</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="6" t="n">
         <v>131.7</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="6" t="n">
         <v>93.5</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="6" t="n">
         <v>126.6</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="6" t="n">
         <v>116.7</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="I5" s="6" t="n">
         <v>124.1</v>
       </c>
-      <c r="J5" s="8" t="n">
+      <c r="J5" s="6" t="n">
         <v>109.2</v>
       </c>
-      <c r="K5" s="8" t="n">
+      <c r="K5" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L5" s="8" t="n">
+      <c r="L5" s="6" t="n">
         <v>112.3</v>
       </c>
-      <c r="M5" s="8" t="n">
+      <c r="M5" s="6" t="n">
         <v>120.9</v>
       </c>
-      <c r="N5" s="8" t="n">
+      <c r="N5" s="6" t="n">
         <v>132.4</v>
       </c>
-      <c r="O5" s="8" t="n">
+      <c r="O5" s="6" t="n">
         <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="A6" s="4" t="n">
         <v>2021</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="n">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="n">
         <v>121.5</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="6" t="n">
         <v>133.4</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="6" t="n">
         <v>127.4</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="6" t="n">
         <v>118.6</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="6" t="n">
         <v>124.6</v>
       </c>
-      <c r="J6" s="8" t="n">
+      <c r="J6" s="6" t="n">
         <v>110</v>
       </c>
-      <c r="K6" s="8" t="n">
+      <c r="K6" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L6" s="8" t="n">
+      <c r="L6" s="6" t="n">
         <v>112.8</v>
       </c>
-      <c r="M6" s="8" t="n">
+      <c r="M6" s="6" t="n">
         <v>121.1</v>
       </c>
-      <c r="N6" s="8" t="n">
+      <c r="N6" s="6" t="n">
         <v>132.9</v>
       </c>
-      <c r="O6" s="8" t="n">
+      <c r="O6" s="6" t="n">
         <v>116.6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="A8" s="4" t="n">
         <v>2021</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="5" t="n">
         <v>121</v>
       </c>
-      <c r="D8" s="8" t="n">
+      <c r="D8" s="6" t="n">
         <v>132.6</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="6" t="n">
         <v>93.3</v>
       </c>
-      <c r="G8" s="8" t="n">
+      <c r="G8" s="6" t="n">
         <v>126.8</v>
       </c>
-      <c r="H8" s="8" t="n">
+      <c r="H8" s="6" t="n">
         <v>117.1</v>
       </c>
-      <c r="I8" s="8" t="n">
+      <c r="I8" s="6" t="n">
         <v>124.4</v>
       </c>
-      <c r="J8" s="8" t="n">
+      <c r="J8" s="6" t="n">
         <v>106.8</v>
       </c>
-      <c r="K8" s="8" t="n">
+      <c r="K8" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L8" s="8" t="n">
+      <c r="L8" s="6" t="n">
         <v>112.5</v>
       </c>
-      <c r="M8" s="8" t="n">
+      <c r="M8" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="N8" s="8" t="n">
+      <c r="N8" s="6" t="n">
         <v>132.5</v>
       </c>
-      <c r="O8" s="8" t="n">
+      <c r="O8" s="6" t="n">
         <v>116.8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="5" t="n">
         <v>121</v>
       </c>
-      <c r="D9" s="8" t="n">
+      <c r="D9" s="6" t="n">
         <v>132.7</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="6" t="n">
         <v>93.3</v>
       </c>
-      <c r="G9" s="8" t="n">
+      <c r="G9" s="6" t="n">
         <v>127.2</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="6" t="n">
         <v>117.3</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="6" t="n">
         <v>124.5</v>
       </c>
-      <c r="J9" s="8" t="n">
+      <c r="J9" s="6" t="n">
         <v>107.1</v>
       </c>
-      <c r="K9" s="8" t="n">
+      <c r="K9" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L9" s="8" t="n">
+      <c r="L9" s="6" t="n">
         <v>112.5</v>
       </c>
-      <c r="M9" s="8" t="n">
+      <c r="M9" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="N9" s="8" t="n">
+      <c r="N9" s="6" t="n">
         <v>132.4</v>
       </c>
-      <c r="O9" s="8" t="n">
+      <c r="O9" s="6" t="n">
         <v>116.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="5" t="n">
         <v>121.2</v>
       </c>
-      <c r="D10" s="8" t="n">
+      <c r="D10" s="6" t="n">
         <v>132.9</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="6" t="n">
         <v>93.3</v>
       </c>
-      <c r="G10" s="8" t="n">
+      <c r="G10" s="6" t="n">
         <v>127.2</v>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="H10" s="6" t="n">
         <v>118</v>
       </c>
-      <c r="I10" s="8" t="n">
+      <c r="I10" s="6" t="n">
         <v>124.6</v>
       </c>
-      <c r="J10" s="8" t="n">
+      <c r="J10" s="6" t="n">
         <v>110.2</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L10" s="8" t="n">
+      <c r="L10" s="6" t="n">
         <v>112.9</v>
       </c>
-      <c r="M10" s="8" t="n">
+      <c r="M10" s="6" t="n">
         <v>120.9</v>
       </c>
-      <c r="N10" s="8" t="n">
+      <c r="N10" s="6" t="n">
         <v>132.5</v>
       </c>
-      <c r="O10" s="8" t="n">
+      <c r="O10" s="6" t="n">
         <v>116.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="5" t="n">
         <v>121.3</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="8" t="n">
         <v>133</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="8" t="n">
         <v>93.2</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="G11" s="8" t="n">
         <v>127.2</v>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="H11" s="8" t="n">
         <v>118.4</v>
       </c>
-      <c r="I11" s="10" t="n">
+      <c r="I11" s="8" t="n">
         <v>124.6</v>
       </c>
-      <c r="J11" s="10" t="n">
+      <c r="J11" s="8" t="n">
         <v>110.6</v>
       </c>
-      <c r="K11" s="10" t="n">
+      <c r="K11" s="8" t="n">
         <v>97.5</v>
       </c>
-      <c r="L11" s="10" t="n">
+      <c r="L11" s="8" t="n">
         <v>113.1</v>
       </c>
-      <c r="M11" s="10" t="n">
+      <c r="M11" s="8" t="n">
         <v>121.1</v>
       </c>
-      <c r="N11" s="10" t="n">
+      <c r="N11" s="8" t="n">
         <v>132.7</v>
       </c>
-      <c r="O11" s="10" t="n">
+      <c r="O11" s="8" t="n">
         <v>116.3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="5" t="n">
         <v>121.4</v>
       </c>
-      <c r="D12" s="8" t="n">
+      <c r="D12" s="6" t="n">
         <v>133.1</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G12" s="8" t="n">
+      <c r="G12" s="6" t="n">
         <v>127.3</v>
       </c>
-      <c r="H12" s="8" t="n">
+      <c r="H12" s="6" t="n">
         <v>118.7</v>
       </c>
-      <c r="I12" s="8" t="n">
+      <c r="I12" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J12" s="8" t="n">
+      <c r="J12" s="6" t="n">
         <v>110.9</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L12" s="8" t="n">
+      <c r="L12" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="M12" s="8" t="n">
+      <c r="M12" s="6" t="n">
         <v>121.1</v>
       </c>
-      <c r="N12" s="8" t="n">
+      <c r="N12" s="6" t="n">
         <v>132.8</v>
       </c>
-      <c r="O12" s="8" t="n">
+      <c r="O12" s="6" t="n">
         <v>116.3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="5" t="n">
         <v>121.4</v>
       </c>
-      <c r="D13" s="8" t="n">
+      <c r="D13" s="6" t="n">
         <v>133.2</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G13" s="8" t="n">
+      <c r="G13" s="6" t="n">
         <v>127.3</v>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H13" s="6" t="n">
         <v>118.7</v>
       </c>
-      <c r="I13" s="8" t="n">
+      <c r="I13" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J13" s="8" t="n">
+      <c r="J13" s="6" t="n">
         <v>110.4</v>
       </c>
-      <c r="K13" s="8" t="n">
+      <c r="K13" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="M13" s="8" t="n">
+      <c r="M13" s="6" t="n">
         <v>121.1</v>
       </c>
-      <c r="N13" s="8" t="n">
+      <c r="N13" s="6" t="n">
         <v>132.8</v>
       </c>
-      <c r="O13" s="8" t="n">
+      <c r="O13" s="6" t="n">
         <v>116.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="5" t="n">
         <v>121.3</v>
       </c>
-      <c r="D14" s="8" t="n">
+      <c r="D14" s="6" t="n">
         <v>133.2</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G14" s="8" t="n">
+      <c r="G14" s="6" t="n">
         <v>127.3</v>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="H14" s="6" t="n">
         <v>118.7</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="I14" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J14" s="8" t="n">
+      <c r="J14" s="6" t="n">
         <v>110.5</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L14" s="8" t="n">
+      <c r="L14" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="M14" s="8" t="n">
+      <c r="M14" s="6" t="n">
         <v>121.1</v>
       </c>
-      <c r="N14" s="8" t="n">
+      <c r="N14" s="6" t="n">
         <v>132.9</v>
       </c>
-      <c r="O14" s="8" t="n">
+      <c r="O14" s="6" t="n">
         <v>116.4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="5" t="n">
         <v>121.5</v>
       </c>
-      <c r="D15" s="8" t="n">
+      <c r="D15" s="6" t="n">
         <v>133.3</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G15" s="8" t="n">
+      <c r="G15" s="6" t="n">
         <v>127.4</v>
       </c>
-      <c r="H15" s="8" t="n">
+      <c r="H15" s="6" t="n">
         <v>118.7</v>
       </c>
-      <c r="I15" s="8" t="n">
+      <c r="I15" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J15" s="8" t="n">
+      <c r="J15" s="6" t="n">
         <v>110.4</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L15" s="8" t="n">
+      <c r="L15" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="M15" s="8" t="n">
+      <c r="M15" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="N15" s="8" t="n">
+      <c r="N15" s="6" t="n">
         <v>132.9</v>
       </c>
-      <c r="O15" s="8" t="n">
+      <c r="O15" s="6" t="n">
         <v>116.4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="5" t="n">
         <v>121.6</v>
       </c>
-      <c r="D16" s="8" t="n">
+      <c r="D16" s="6" t="n">
         <v>133.5</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G16" s="8" t="n">
+      <c r="G16" s="6" t="n">
         <v>127.5</v>
       </c>
-      <c r="H16" s="8" t="n">
+      <c r="H16" s="6" t="n">
         <v>118.8</v>
       </c>
-      <c r="I16" s="8" t="n">
+      <c r="I16" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J16" s="8" t="n">
+      <c r="J16" s="6" t="n">
         <v>110.5</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L16" s="8" t="n">
+      <c r="L16" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="M16" s="8" t="n">
+      <c r="M16" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="N16" s="8" t="n">
+      <c r="N16" s="6" t="n">
         <v>132.7</v>
       </c>
-      <c r="O16" s="8" t="n">
+      <c r="O16" s="6" t="n">
         <v>116.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="5" t="n">
         <v>121.6</v>
       </c>
-      <c r="D17" s="8" t="n">
+      <c r="D17" s="6" t="n">
         <v>133.8</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="8" t="n">
+      <c r="F17" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G17" s="8" t="n">
+      <c r="G17" s="6" t="n">
         <v>127.5</v>
       </c>
-      <c r="H17" s="8" t="n">
+      <c r="H17" s="6" t="n">
         <v>119.3</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="I17" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J17" s="8" t="n">
+      <c r="J17" s="6" t="n">
         <v>110.8</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L17" s="8" t="n">
+      <c r="L17" s="6" t="n">
         <v>112.6</v>
       </c>
-      <c r="M17" s="8" t="n">
+      <c r="M17" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="N17" s="8" t="n">
+      <c r="N17" s="6" t="n">
         <v>133.1</v>
       </c>
-      <c r="O17" s="8" t="n">
+      <c r="O17" s="6" t="n">
         <v>116.8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="5" t="n">
         <v>122</v>
       </c>
-      <c r="D18" s="8" t="n">
+      <c r="D18" s="6" t="n">
         <v>134.4</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="8" t="n">
+      <c r="F18" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G18" s="8" t="n">
+      <c r="G18" s="6" t="n">
         <v>127.8</v>
       </c>
-      <c r="H18" s="8" t="n">
+      <c r="H18" s="6" t="n">
         <v>119.7</v>
       </c>
-      <c r="I18" s="8" t="n">
+      <c r="I18" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J18" s="8" t="n">
+      <c r="J18" s="6" t="n">
         <v>110.4</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L18" s="8" t="n">
+      <c r="L18" s="6" t="n">
         <v>112.6</v>
       </c>
-      <c r="M18" s="8" t="n">
+      <c r="M18" s="6" t="n">
         <v>121.1</v>
       </c>
-      <c r="N18" s="8" t="n">
+      <c r="N18" s="6" t="n">
         <v>133.5</v>
       </c>
-      <c r="O18" s="8" t="n">
+      <c r="O18" s="6" t="n">
         <v>117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="5" t="n">
         <v>122.2</v>
       </c>
-      <c r="D19" s="8" t="n">
+      <c r="D19" s="6" t="n">
         <v>135.2</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="8" t="n">
+      <c r="F19" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G19" s="8" t="n">
+      <c r="G19" s="6" t="n">
         <v>127.9</v>
       </c>
-      <c r="H19" s="8" t="n">
+      <c r="H19" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="I19" s="8" t="n">
+      <c r="I19" s="6" t="n">
         <v>124.7</v>
       </c>
-      <c r="J19" s="8" t="n">
+      <c r="J19" s="6" t="n">
         <v>111.7</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L19" s="8" t="n">
+      <c r="L19" s="6" t="n">
         <v>112.9</v>
       </c>
-      <c r="M19" s="8" t="n">
+      <c r="M19" s="6" t="n">
         <v>121.2</v>
       </c>
-      <c r="N19" s="8" t="n">
+      <c r="N19" s="6" t="n">
         <v>134</v>
       </c>
-      <c r="O19" s="8" t="n">
+      <c r="O19" s="6" t="n">
         <v>117.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <f aca="false">AVERAGE(C8:C19)</f>
         <v>121.458333333333</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <f aca="false">AVERAGE(D8:D19)</f>
         <v>133.408333333333</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <f aca="false">AVERAGE(F8:F19)</f>
         <v>93.125</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <f aca="false">AVERAGE(G8:G19)</f>
         <v>127.366666666667</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <f aca="false">AVERAGE(H8:H19)</f>
         <v>118.616666666667</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="1" t="n">
         <f aca="false">AVERAGE(I8:I19)</f>
         <v>124.641666666667</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="1" t="n">
         <f aca="false">AVERAGE(J8:J19)</f>
         <v>110.025</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="1" t="n">
         <f aca="false">AVERAGE(K8:K19)</f>
         <v>97.5</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20" s="1" t="n">
         <f aca="false">AVERAGE(L8:L19)</f>
         <v>112.841666666667</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <f aca="false">AVERAGE(M8:M19)</f>
         <v>121.05</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="1" t="n">
         <f aca="false">AVERAGE(N8:N19)</f>
         <v>132.9</v>
       </c>
-      <c r="O20" s="13" t="n">
+      <c r="O20" s="11" t="n">
         <f aca="false">AVERAGE(O8:O19)</f>
         <v>116.558333333333</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="n">
+      <c r="A22" s="4" t="n">
         <v>2022</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="5" t="n">
         <f aca="false">C8+1.9</f>
         <v>122.9</v>
       </c>
-      <c r="D22" s="8" t="n">
+      <c r="D22" s="6" t="n">
         <v>136.3</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="8" t="n">
+      <c r="F22" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G22" s="8" t="n">
+      <c r="G22" s="6" t="n">
         <v>127.9</v>
       </c>
-      <c r="H22" s="8" t="n">
+      <c r="H22" s="6" t="n">
         <v>120.7</v>
       </c>
-      <c r="I22" s="8" t="n">
+      <c r="I22" s="6" t="n">
         <v>124.8</v>
       </c>
-      <c r="J22" s="8" t="n">
+      <c r="J22" s="6" t="n">
         <f aca="false">J8+3.5</f>
         <v>110.3</v>
       </c>
-      <c r="K22" s="8" t="n">
+      <c r="K22" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L22" s="8" t="n">
+      <c r="L22" s="6" t="n">
         <v>113.8</v>
       </c>
-      <c r="M22" s="8" t="n">
+      <c r="M22" s="6" t="n">
         <v>121.8</v>
       </c>
-      <c r="N22" s="8" t="n">
+      <c r="N22" s="6" t="n">
         <v>135.3</v>
       </c>
-      <c r="O22" s="8" t="n">
+      <c r="O22" s="6" t="n">
         <v>117.5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="5" t="n">
         <v>123.2</v>
       </c>
-      <c r="D23" s="8" t="n">
+      <c r="D23" s="6" t="n">
         <v>136.9</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="8" t="n">
+      <c r="F23" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G23" s="8" t="n">
+      <c r="G23" s="6" t="n">
         <v>128.4</v>
       </c>
-      <c r="H23" s="8" t="n">
+      <c r="H23" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="I23" s="8" t="n">
+      <c r="I23" s="6" t="n">
         <v>125.1</v>
       </c>
-      <c r="J23" s="8" t="n">
+      <c r="J23" s="6" t="n">
         <v>110.8</v>
       </c>
-      <c r="K23" s="8" t="n">
+      <c r="K23" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L23" s="8" t="n">
+      <c r="L23" s="6" t="n">
         <v>114.3</v>
       </c>
-      <c r="M23" s="8" t="n">
+      <c r="M23" s="6" t="n">
         <v>121.9</v>
       </c>
-      <c r="N23" s="8" t="n">
+      <c r="N23" s="6" t="n">
         <v>135.8</v>
       </c>
-      <c r="O23" s="8" t="n">
+      <c r="O23" s="6" t="n">
         <v>117.7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="4"/>
+      <c r="B24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="5" t="n">
         <f aca="false">C10+2.4</f>
         <v>123.6</v>
       </c>
-      <c r="D24" s="8" t="n">
+      <c r="D24" s="6" t="n">
         <v>137.5</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="8" t="n">
+      <c r="F24" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G24" s="8" t="n">
+      <c r="G24" s="6" t="n">
         <v>128.4</v>
       </c>
-      <c r="H24" s="8" t="n">
+      <c r="H24" s="6" t="n">
         <v>121.5</v>
       </c>
-      <c r="I24" s="8" t="n">
+      <c r="I24" s="6" t="n">
         <v>124.8</v>
       </c>
-      <c r="J24" s="8" t="n">
+      <c r="J24" s="6" t="n">
         <f aca="false">J10+4.3</f>
         <v>114.5</v>
       </c>
-      <c r="K24" s="8" t="n">
+      <c r="K24" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L24" s="8" t="n">
+      <c r="L24" s="6" t="n">
         <v>114.1</v>
       </c>
-      <c r="M24" s="8" t="n">
+      <c r="M24" s="6" t="n">
         <v>122</v>
       </c>
-      <c r="N24" s="8" t="n">
+      <c r="N24" s="6" t="n">
         <v>136.4</v>
       </c>
-      <c r="O24" s="8" t="n">
+      <c r="O24" s="6" t="n">
         <v>118.4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="5" t="n">
         <v>123.8</v>
       </c>
-      <c r="D25" s="8" t="n">
+      <c r="D25" s="6" t="n">
         <v>138.1</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="8" t="n">
+      <c r="F25" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="G25" s="8" t="n">
+      <c r="G25" s="6" t="n">
         <v>128.5</v>
       </c>
-      <c r="H25" s="8" t="n">
+      <c r="H25" s="6" t="n">
         <v>121.6</v>
       </c>
-      <c r="I25" s="8" t="n">
+      <c r="I25" s="6" t="n">
         <v>124.9</v>
       </c>
-      <c r="J25" s="8" t="n">
+      <c r="J25" s="6" t="n">
         <v>115.2</v>
       </c>
-      <c r="K25" s="8" t="n">
+      <c r="K25" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L25" s="8" t="n">
+      <c r="L25" s="6" t="n">
         <v>114.6</v>
       </c>
-      <c r="M25" s="8" t="n">
+      <c r="M25" s="6" t="n">
         <v>122.3</v>
       </c>
-      <c r="N25" s="8" t="n">
+      <c r="N25" s="6" t="n">
         <v>136.9</v>
       </c>
-      <c r="O25" s="8" t="n">
+      <c r="O25" s="6" t="n">
         <v>118.4</v>
       </c>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="4"/>
+      <c r="B26" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="5" t="n">
         <v>124.3</v>
       </c>
-      <c r="D26" s="8" t="n">
+      <c r="D26" s="6" t="n">
         <v>139</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="8" t="n">
+      <c r="F26" s="6" t="n">
         <v>93.1</v>
       </c>
-      <c r="G26" s="8" t="n">
+      <c r="G26" s="6" t="n">
         <v>129</v>
       </c>
-      <c r="H26" s="8" t="n">
+      <c r="H26" s="6" t="n">
         <v>122.2</v>
       </c>
-      <c r="I26" s="8" t="n">
+      <c r="I26" s="6" t="n">
         <v>125.2</v>
       </c>
-      <c r="J26" s="8" t="n">
+      <c r="J26" s="6" t="n">
         <v>116.1</v>
       </c>
-      <c r="K26" s="8" t="n">
+      <c r="K26" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L26" s="8" t="n">
+      <c r="L26" s="6" t="n">
         <v>115</v>
       </c>
-      <c r="M26" s="8" t="n">
+      <c r="M26" s="6" t="n">
         <v>122.3</v>
       </c>
-      <c r="N26" s="8" t="n">
+      <c r="N26" s="6" t="n">
         <v>137.7</v>
       </c>
-      <c r="O26" s="8" t="n">
+      <c r="O26" s="6" t="n">
         <v>118.5</v>
       </c>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="5" t="n">
         <f aca="false">C13+3.6</f>
         <v>125</v>
       </c>
-      <c r="D27" s="8" t="n">
+      <c r="D27" s="6" t="n">
         <v>140.6</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="8" t="n">
+      <c r="F27" s="6" t="n">
         <v>93.3</v>
       </c>
-      <c r="G27" s="8" t="n">
+      <c r="G27" s="6" t="n">
         <v>129.1</v>
       </c>
-      <c r="H27" s="8" t="n">
+      <c r="H27" s="6" t="n">
         <v>122.7</v>
       </c>
-      <c r="I27" s="8" t="n">
+      <c r="I27" s="6" t="n">
         <v>125.4</v>
       </c>
-      <c r="J27" s="8" t="n">
+      <c r="J27" s="6" t="n">
         <f aca="false">J13+5.7</f>
         <v>116.1</v>
       </c>
-      <c r="K27" s="8" t="n">
+      <c r="K27" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L27" s="8" t="n">
+      <c r="L27" s="6" t="n">
         <v>115.5</v>
       </c>
-      <c r="M27" s="8" t="n">
+      <c r="M27" s="6" t="n">
         <v>122.4</v>
       </c>
-      <c r="N27" s="8" t="n">
+      <c r="N27" s="6" t="n">
         <v>139.5</v>
       </c>
-      <c r="O27" s="8" t="n">
+      <c r="O27" s="6" t="n">
         <v>119</v>
       </c>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="4"/>
+      <c r="B28" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="5" t="n">
         <f aca="false">C14+4.1</f>
         <v>125.4</v>
       </c>
-      <c r="D28" s="8" t="n">
+      <c r="D28" s="6" t="n">
         <v>142.2</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="8" t="n">
+      <c r="F28" s="6" t="n">
         <v>93.4</v>
       </c>
-      <c r="G28" s="8" t="n">
+      <c r="G28" s="6" t="n">
         <v>129.1</v>
       </c>
-      <c r="H28" s="8" t="n">
+      <c r="H28" s="6" t="n">
         <v>123.4</v>
       </c>
-      <c r="I28" s="8" t="n">
+      <c r="I28" s="6" t="n">
         <v>125.7</v>
       </c>
-      <c r="J28" s="8" t="n">
+      <c r="J28" s="6" t="n">
         <f aca="false">J14+6.7</f>
         <v>117.2</v>
       </c>
-      <c r="K28" s="8" t="n">
+      <c r="K28" s="6" t="n">
         <v>97.5</v>
       </c>
-      <c r="L28" s="8" t="n">
+      <c r="L28" s="6" t="n">
         <v>115.8</v>
       </c>
-      <c r="M28" s="8" t="n">
+      <c r="M28" s="6" t="n">
         <v>122.5</v>
       </c>
-      <c r="N28" s="8" t="n">
+      <c r="N28" s="6" t="n">
         <v>140.6</v>
       </c>
-      <c r="O28" s="8" t="n">
+      <c r="O28" s="6" t="n">
         <v>118.9</v>
       </c>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="4"/>
+      <c r="B29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="5" t="n">
         <f aca="false">C15+4.6</f>
         <v>126.1</v>
       </c>
-      <c r="D29" s="15" t="n">
+      <c r="D29" s="13" t="n">
         <v>143</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="15" t="n">
+      <c r="F29" s="13" t="n">
         <v>93.4</v>
       </c>
-      <c r="G29" s="15" t="n">
+      <c r="G29" s="13" t="n">
         <v>129.8</v>
       </c>
-      <c r="H29" s="15" t="n">
+      <c r="H29" s="13" t="n">
         <v>123.8</v>
       </c>
-      <c r="I29" s="15" t="n">
+      <c r="I29" s="13" t="n">
         <v>125.8</v>
       </c>
-      <c r="J29" s="15" t="n">
+      <c r="J29" s="13" t="n">
         <f aca="false">J15+7.4</f>
         <v>117.8</v>
       </c>
-      <c r="K29" s="15" t="n">
+      <c r="K29" s="13" t="n">
         <v>97.5</v>
       </c>
-      <c r="L29" s="15" t="n">
+      <c r="L29" s="13" t="n">
         <v>116.1</v>
       </c>
-      <c r="M29" s="15" t="n">
+      <c r="M29" s="13" t="n">
         <v>122.5</v>
       </c>
-      <c r="N29" s="15" t="n">
+      <c r="N29" s="13" t="n">
         <v>141.4</v>
       </c>
-      <c r="O29" s="15" t="n">
+      <c r="O29" s="13" t="n">
         <v>119.2</v>
       </c>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <f aca="false">AVERAGE(C22:C29)</f>
         <v>124.2875</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <f aca="false">AVERAGE(D22:D29)</f>
         <v>139.2</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <f aca="false">AVERAGE(F22:F29)</f>
         <v>93.1625</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <f aca="false">AVERAGE(G22:G29)</f>
         <v>128.775</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <f aca="false">AVERAGE(H22:H29)</f>
         <v>122.1125</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="I30" s="1" t="n">
         <f aca="false">AVERAGE(I22:I29)</f>
         <v>125.2125</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="J30" s="1" t="n">
         <f aca="false">AVERAGE(J22:J29)</f>
         <v>114.75</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="K30" s="1" t="n">
         <f aca="false">AVERAGE(K22:K29)</f>
         <v>97.5</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="L30" s="1" t="n">
         <f aca="false">AVERAGE(L22:L29)</f>
         <v>114.9</v>
       </c>
-      <c r="M30" s="0" t="n">
+      <c r="M30" s="1" t="n">
         <f aca="false">AVERAGE(M22:M29)</f>
         <v>122.2125</v>
       </c>
-      <c r="N30" s="0" t="n">
+      <c r="N30" s="1" t="n">
         <f aca="false">AVERAGE(N22:N29)</f>
         <v>137.95</v>
       </c>
-      <c r="O30" s="0" t="n">
+      <c r="O30" s="1" t="n">
         <f aca="false">AVERAGE(O22:O29)</f>
         <v>118.45</v>
       </c>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="7"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-    </row>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -37915,4 +37937,476 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="n">
+        <v>44773</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="15" t="n">
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="n">
+        <v>44592</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="n">
+        <v>44408</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="n">
+        <v>44043</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="n">
+        <v>43861</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="n">
+        <v>43677</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2006</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="n">
+        <v>43496</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9.05</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14" t="n">
+        <v>43312</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>8.45</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="14" t="n">
+        <v>43131</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>6.77</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="n">
+        <v>42947</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="n">
+        <v>42766</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="n">
+        <v>42582</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="n">
+        <v>42400</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="n">
+        <v>42216</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="n">
+        <v>42035</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>7.63</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="n">
+        <v>41851</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>7.63</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="n">
+        <v>41670</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="n">
+        <v>41486</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>8.45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
+        <v>41305</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>7.95</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="n">
+        <v>41121</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="n">
+        <v>40939</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="n">
+        <v>40755</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="n">
+        <v>40390</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="n">
+        <v>40209</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="n">
+        <v>40025</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>6.77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="n">
+        <v>39629</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="n">
+        <v>39263</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="n">
+        <v>39113</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="n">
+        <v>38868</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="n">
+        <v>38748</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="n">
+        <v>38533</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="n">
+        <v>38138</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="n">
+        <v>37741</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="n">
+        <v>37376</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="n">
+        <v>37011</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="n">
+        <v>36646</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>4.52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ xkre/malaysia-inflation-calc@67fb366f254fdaf2c01ce39d36758e5f785527e0 🚀
</commit_message>
<xml_diff>
--- a/data/CpiDataset.xlsx
+++ b/data/CpiDataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arekr\source\repos\malaysia-inflation-calc\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62A1E61-DCC4-4AC0-9D32-8D3D162F559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8891B665-D26A-4819-9C97-4D8C809E1069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Malaysia" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7469" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7789" uniqueCount="86">
   <si>
     <t>Period type</t>
   </si>
@@ -1248,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD297"/>
+  <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView topLeftCell="C254" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H286" sqref="H286"/>
+    <sheetView topLeftCell="A260" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E296" sqref="E296:E308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -6170,7 +6170,7 @@
         <v>169.2</v>
       </c>
     </row>
-    <row r="273" spans="1:30">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>6</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>93.1</v>
       </c>
     </row>
-    <row r="274" spans="1:30">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>6</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="275" spans="1:30">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>6</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>118.6</v>
       </c>
     </row>
-    <row r="276" spans="1:30">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>6</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>124.6</v>
       </c>
     </row>
-    <row r="277" spans="1:30">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>6</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>113.9</v>
       </c>
     </row>
-    <row r="278" spans="1:30">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>6</v>
       </c>
@@ -6271,50 +6271,8 @@
       <c r="E278">
         <v>97.5</v>
       </c>
-      <c r="L278">
-        <v>123.1</v>
-      </c>
-      <c r="M278">
-        <v>137.1</v>
-      </c>
-      <c r="N278">
-        <v>169.2</v>
-      </c>
-      <c r="O278">
-        <v>93.1</v>
-      </c>
-      <c r="P278">
-        <v>121</v>
-      </c>
-      <c r="Q278">
-        <v>118.6</v>
-      </c>
-      <c r="R278">
-        <v>124.6</v>
-      </c>
-      <c r="S278">
-        <v>113.9</v>
-      </c>
-      <c r="T278">
-        <v>97.5</v>
-      </c>
-      <c r="U278">
-        <v>112.8</v>
-      </c>
-      <c r="V278">
-        <v>121.1</v>
-      </c>
-      <c r="W278">
-        <v>132.9</v>
-      </c>
-      <c r="X278">
-        <v>116.6</v>
-      </c>
-      <c r="Y278">
-        <v>113.9</v>
-      </c>
-    </row>
-    <row r="279" spans="1:30">
+    </row>
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>6</v>
       </c>
@@ -6330,47 +6288,8 @@
       <c r="E279">
         <v>112.8</v>
       </c>
-      <c r="L279">
-        <v>127.21666666666665</v>
-      </c>
-      <c r="M279">
-        <v>145.01666666666665</v>
-      </c>
-      <c r="N279">
-        <v>170.11666666666665</v>
-      </c>
-      <c r="O279">
-        <v>93.241666666666674</v>
-      </c>
-      <c r="P279">
-        <v>123.21666666666668</v>
-      </c>
-      <c r="Q279">
-        <v>122.81666666666668</v>
-      </c>
-      <c r="R279">
-        <v>125.52500000000002</v>
-      </c>
-      <c r="S279">
-        <v>119.24166666666667</v>
-      </c>
-      <c r="T279">
-        <v>97.491666666666674</v>
-      </c>
-      <c r="U279">
-        <v>115.35833333333331</v>
-      </c>
-      <c r="V279">
-        <v>122.40000000000002</v>
-      </c>
-      <c r="W279">
-        <v>139.53333333333333</v>
-      </c>
-      <c r="X279">
-        <v>118.86666666666667</v>
-      </c>
-    </row>
-    <row r="280" spans="1:30">
+    </row>
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>6</v>
       </c>
@@ -6387,7 +6306,7 @@
         <v>121.1</v>
       </c>
     </row>
-    <row r="281" spans="1:30">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>6</v>
       </c>
@@ -6404,7 +6323,7 @@
         <v>132.9</v>
       </c>
     </row>
-    <row r="282" spans="1:30">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>6</v>
       </c>
@@ -6421,7 +6340,7 @@
         <v>116.6</v>
       </c>
     </row>
-    <row r="283" spans="1:30">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
         <v>6</v>
       </c>
@@ -6437,53 +6356,8 @@
       <c r="E283">
         <v>127.21666666666665</v>
       </c>
-      <c r="K283">
-        <v>123.1</v>
-      </c>
-      <c r="L283">
-        <v>127.21666666666665</v>
-      </c>
-      <c r="R283">
-        <v>127.21666666666665</v>
-      </c>
-      <c r="S283">
-        <v>145.01666666666665</v>
-      </c>
-      <c r="T283">
-        <v>170.11666666666665</v>
-      </c>
-      <c r="U283">
-        <v>93.241666666666674</v>
-      </c>
-      <c r="V283">
-        <v>123.21666666666668</v>
-      </c>
-      <c r="W283">
-        <v>122.81666666666668</v>
-      </c>
-      <c r="X283">
-        <v>125.52500000000002</v>
-      </c>
-      <c r="Y283">
-        <v>119.24166666666667</v>
-      </c>
-      <c r="Z283">
-        <v>97.491666666666674</v>
-      </c>
-      <c r="AA283">
-        <v>115.35833333333331</v>
-      </c>
-      <c r="AB283">
-        <v>122.40000000000002</v>
-      </c>
-      <c r="AC283">
-        <v>139.53333333333333</v>
-      </c>
-      <c r="AD283">
-        <v>118.86666666666667</v>
-      </c>
-    </row>
-    <row r="284" spans="1:30">
+    </row>
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
         <v>6</v>
       </c>
@@ -6499,14 +6373,8 @@
       <c r="E284">
         <v>145.01666666666665</v>
       </c>
-      <c r="K284">
-        <v>137.1</v>
-      </c>
-      <c r="L284">
-        <v>145.01666666666665</v>
-      </c>
-    </row>
-    <row r="285" spans="1:30">
+    </row>
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>6</v>
       </c>
@@ -6522,17 +6390,8 @@
       <c r="E285">
         <v>170.11666666666665</v>
       </c>
-      <c r="K285">
-        <v>169.2</v>
-      </c>
-      <c r="L285">
-        <v>170.11666666666665</v>
-      </c>
-      <c r="R285">
-        <v>127.21666666666665</v>
-      </c>
-    </row>
-    <row r="286" spans="1:30">
+    </row>
+    <row r="286" spans="1:5">
       <c r="A286" t="s">
         <v>6</v>
       </c>
@@ -6548,17 +6407,8 @@
       <c r="E286">
         <v>93.241666666666674</v>
       </c>
-      <c r="K286">
-        <v>93.1</v>
-      </c>
-      <c r="L286">
-        <v>93.241666666666674</v>
-      </c>
-      <c r="R286">
-        <v>145.01666666666665</v>
-      </c>
-    </row>
-    <row r="287" spans="1:30">
+    </row>
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
         <v>6</v>
       </c>
@@ -6574,17 +6424,8 @@
       <c r="E287">
         <v>123.21666666666668</v>
       </c>
-      <c r="K287">
-        <v>121</v>
-      </c>
-      <c r="L287">
-        <v>123.21666666666668</v>
-      </c>
-      <c r="R287">
-        <v>170.11666666666665</v>
-      </c>
-    </row>
-    <row r="288" spans="1:30">
+    </row>
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>6</v>
       </c>
@@ -6600,17 +6441,8 @@
       <c r="E288">
         <v>122.81666666666668</v>
       </c>
-      <c r="K288">
-        <v>118.6</v>
-      </c>
-      <c r="L288">
-        <v>122.81666666666668</v>
-      </c>
-      <c r="R288">
-        <v>93.241666666666674</v>
-      </c>
-    </row>
-    <row r="289" spans="1:18">
+    </row>
+    <row r="289" spans="1:5">
       <c r="A289" t="s">
         <v>6</v>
       </c>
@@ -6626,17 +6458,8 @@
       <c r="E289">
         <v>125.52500000000002</v>
       </c>
-      <c r="K289">
-        <v>124.6</v>
-      </c>
-      <c r="L289">
-        <v>125.52500000000002</v>
-      </c>
-      <c r="R289">
-        <v>123.21666666666668</v>
-      </c>
-    </row>
-    <row r="290" spans="1:18">
+    </row>
+    <row r="290" spans="1:5">
       <c r="A290" t="s">
         <v>6</v>
       </c>
@@ -6652,17 +6475,8 @@
       <c r="E290">
         <v>119.24166666666667</v>
       </c>
-      <c r="K290">
-        <v>113.9</v>
-      </c>
-      <c r="L290">
-        <v>119.24166666666667</v>
-      </c>
-      <c r="R290">
-        <v>122.81666666666668</v>
-      </c>
-    </row>
-    <row r="291" spans="1:18">
+    </row>
+    <row r="291" spans="1:5">
       <c r="A291" t="s">
         <v>6</v>
       </c>
@@ -6678,17 +6492,8 @@
       <c r="E291">
         <v>97.491666666666674</v>
       </c>
-      <c r="K291">
-        <v>97.5</v>
-      </c>
-      <c r="L291">
-        <v>97.491666666666674</v>
-      </c>
-      <c r="R291">
-        <v>125.52500000000002</v>
-      </c>
-    </row>
-    <row r="292" spans="1:18">
+    </row>
+    <row r="292" spans="1:5">
       <c r="A292" t="s">
         <v>6</v>
       </c>
@@ -6704,17 +6509,8 @@
       <c r="E292">
         <v>115.35833333333331</v>
       </c>
-      <c r="K292">
-        <v>112.8</v>
-      </c>
-      <c r="L292">
-        <v>115.35833333333331</v>
-      </c>
-      <c r="R292">
-        <v>119.24166666666667</v>
-      </c>
-    </row>
-    <row r="293" spans="1:18">
+    </row>
+    <row r="293" spans="1:5">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -6730,17 +6526,8 @@
       <c r="E293">
         <v>122.40000000000002</v>
       </c>
-      <c r="K293">
-        <v>121.1</v>
-      </c>
-      <c r="L293">
-        <v>122.40000000000002</v>
-      </c>
-      <c r="R293">
-        <v>97.491666666666674</v>
-      </c>
-    </row>
-    <row r="294" spans="1:18">
+    </row>
+    <row r="294" spans="1:5">
       <c r="A294" t="s">
         <v>6</v>
       </c>
@@ -6756,17 +6543,8 @@
       <c r="E294">
         <v>139.53333333333333</v>
       </c>
-      <c r="K294">
-        <v>132.9</v>
-      </c>
-      <c r="L294">
-        <v>139.53333333333333</v>
-      </c>
-      <c r="R294">
-        <v>115.35833333333331</v>
-      </c>
-    </row>
-    <row r="295" spans="1:18">
+    </row>
+    <row r="295" spans="1:5">
       <c r="A295" t="s">
         <v>6</v>
       </c>
@@ -6782,24 +6560,226 @@
       <c r="E295">
         <v>118.86666666666667</v>
       </c>
-      <c r="K295">
-        <v>116.6</v>
-      </c>
-      <c r="L295">
-        <v>118.86666666666667</v>
-      </c>
-      <c r="R295">
-        <v>122.40000000000002</v>
-      </c>
-    </row>
-    <row r="296" spans="1:18">
-      <c r="R296">
-        <v>139.53333333333333</v>
-      </c>
-    </row>
-    <row r="297" spans="1:18">
-      <c r="R297">
-        <v>118.86666666666667</v>
+    </row>
+    <row r="296" spans="1:5">
+      <c r="A296" t="s">
+        <v>6</v>
+      </c>
+      <c r="B296" t="s">
+        <v>7</v>
+      </c>
+      <c r="C296">
+        <v>2023</v>
+      </c>
+      <c r="D296" t="s">
+        <v>8</v>
+      </c>
+      <c r="E296">
+        <v>130.37500000000003</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" t="s">
+        <v>6</v>
+      </c>
+      <c r="B297" t="s">
+        <v>7</v>
+      </c>
+      <c r="C297">
+        <v>2023</v>
+      </c>
+      <c r="D297" t="s">
+        <v>18</v>
+      </c>
+      <c r="E297">
+        <v>151.98333333333329</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" t="s">
+        <v>6</v>
+      </c>
+      <c r="B298" t="s">
+        <v>7</v>
+      </c>
+      <c r="C298">
+        <v>2023</v>
+      </c>
+      <c r="D298" t="s">
+        <v>19</v>
+      </c>
+      <c r="E298">
+        <v>171.24166666666667</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" t="s">
+        <v>6</v>
+      </c>
+      <c r="B299" t="s">
+        <v>7</v>
+      </c>
+      <c r="C299">
+        <v>2023</v>
+      </c>
+      <c r="D299" t="s">
+        <v>20</v>
+      </c>
+      <c r="E299">
+        <v>93.458333333333329</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" t="s">
+        <v>6</v>
+      </c>
+      <c r="B300" t="s">
+        <v>7</v>
+      </c>
+      <c r="C300">
+        <v>2023</v>
+      </c>
+      <c r="D300" t="s">
+        <v>21</v>
+      </c>
+      <c r="E300">
+        <v>125.25833333333333</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" t="s">
+        <v>6</v>
+      </c>
+      <c r="B301" t="s">
+        <v>7</v>
+      </c>
+      <c r="C301">
+        <v>2023</v>
+      </c>
+      <c r="D301" t="s">
+        <v>22</v>
+      </c>
+      <c r="E301">
+        <v>125.60833333333333</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" t="s">
+        <v>6</v>
+      </c>
+      <c r="B302" t="s">
+        <v>7</v>
+      </c>
+      <c r="C302">
+        <v>2023</v>
+      </c>
+      <c r="D302" t="s">
+        <v>23</v>
+      </c>
+      <c r="E302">
+        <v>128.16666666666666</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" t="s">
+        <v>6</v>
+      </c>
+      <c r="B303" t="s">
+        <v>7</v>
+      </c>
+      <c r="C303">
+        <v>2023</v>
+      </c>
+      <c r="D303" t="s">
+        <v>24</v>
+      </c>
+      <c r="E303">
+        <v>120.50000000000001</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" t="s">
+        <v>6</v>
+      </c>
+      <c r="B304" t="s">
+        <v>7</v>
+      </c>
+      <c r="C304">
+        <v>2023</v>
+      </c>
+      <c r="D304" t="s">
+        <v>25</v>
+      </c>
+      <c r="E304">
+        <v>94.641666666666666</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" t="s">
+        <v>6</v>
+      </c>
+      <c r="B305" t="s">
+        <v>7</v>
+      </c>
+      <c r="C305">
+        <v>2023</v>
+      </c>
+      <c r="D305" t="s">
+        <v>26</v>
+      </c>
+      <c r="E305">
+        <v>117.00833333333333</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" t="s">
+        <v>6</v>
+      </c>
+      <c r="B306" t="s">
+        <v>7</v>
+      </c>
+      <c r="C306">
+        <v>2023</v>
+      </c>
+      <c r="D306" t="s">
+        <v>27</v>
+      </c>
+      <c r="E306">
+        <v>124.66666666666664</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" t="s">
+        <v>6</v>
+      </c>
+      <c r="B307" t="s">
+        <v>7</v>
+      </c>
+      <c r="C307">
+        <v>2023</v>
+      </c>
+      <c r="D307" t="s">
+        <v>28</v>
+      </c>
+      <c r="E307">
+        <v>147.24999999999997</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" t="s">
+        <v>6</v>
+      </c>
+      <c r="B308" t="s">
+        <v>7</v>
+      </c>
+      <c r="C308">
+        <v>2023</v>
+      </c>
+      <c r="D308" t="s">
+        <v>17</v>
+      </c>
+      <c r="E308">
+        <v>121.78333333333332</v>
       </c>
     </row>
   </sheetData>
@@ -6810,10 +6790,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F295"/>
+  <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView topLeftCell="D253" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E283" sqref="E283:E295"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S276" sqref="S276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -12083,6 +12063,227 @@
         <v>119.27499999999998</v>
       </c>
     </row>
+    <row r="296" spans="1:5">
+      <c r="A296" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C296" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E296">
+        <v>131.65833333333333</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" t="s">
+        <v>6</v>
+      </c>
+      <c r="B297" t="s">
+        <v>29</v>
+      </c>
+      <c r="C297" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D297" t="s">
+        <v>18</v>
+      </c>
+      <c r="E297">
+        <v>154.13333333333333</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" t="s">
+        <v>6</v>
+      </c>
+      <c r="B298" t="s">
+        <v>29</v>
+      </c>
+      <c r="C298" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D298" t="s">
+        <v>19</v>
+      </c>
+      <c r="E298">
+        <v>173.04166666666666</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" t="s">
+        <v>6</v>
+      </c>
+      <c r="B299" t="s">
+        <v>29</v>
+      </c>
+      <c r="C299" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D299" t="s">
+        <v>20</v>
+      </c>
+      <c r="E299">
+        <v>93.916666666666671</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" t="s">
+        <v>6</v>
+      </c>
+      <c r="B300" t="s">
+        <v>29</v>
+      </c>
+      <c r="C300" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D300" t="s">
+        <v>21</v>
+      </c>
+      <c r="E300">
+        <v>127.71666666666668</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" t="s">
+        <v>6</v>
+      </c>
+      <c r="B301" t="s">
+        <v>29</v>
+      </c>
+      <c r="C301" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D301" t="s">
+        <v>22</v>
+      </c>
+      <c r="E301">
+        <v>127.24166666666667</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" t="s">
+        <v>6</v>
+      </c>
+      <c r="B302" t="s">
+        <v>29</v>
+      </c>
+      <c r="C302" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D302" t="s">
+        <v>23</v>
+      </c>
+      <c r="E302">
+        <v>127.74166666666666</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" t="s">
+        <v>6</v>
+      </c>
+      <c r="B303" t="s">
+        <v>29</v>
+      </c>
+      <c r="C303" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D303" t="s">
+        <v>24</v>
+      </c>
+      <c r="E303">
+        <v>120.68333333333334</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" t="s">
+        <v>6</v>
+      </c>
+      <c r="B304" t="s">
+        <v>29</v>
+      </c>
+      <c r="C304" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D304" t="s">
+        <v>25</v>
+      </c>
+      <c r="E304">
+        <v>94.441666666666677</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" t="s">
+        <v>6</v>
+      </c>
+      <c r="B305" t="s">
+        <v>29</v>
+      </c>
+      <c r="C305" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D305" t="s">
+        <v>26</v>
+      </c>
+      <c r="E305">
+        <v>117.44166666666666</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" t="s">
+        <v>6</v>
+      </c>
+      <c r="B306" t="s">
+        <v>29</v>
+      </c>
+      <c r="C306" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D306" t="s">
+        <v>27</v>
+      </c>
+      <c r="E306">
+        <v>125.51666666666667</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" t="s">
+        <v>6</v>
+      </c>
+      <c r="B307" t="s">
+        <v>29</v>
+      </c>
+      <c r="C307" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D307" t="s">
+        <v>28</v>
+      </c>
+      <c r="E307">
+        <v>147.30833333333334</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" t="s">
+        <v>6</v>
+      </c>
+      <c r="B308" t="s">
+        <v>29</v>
+      </c>
+      <c r="C308" s="18">
+        <v>2023</v>
+      </c>
+      <c r="D308" t="s">
+        <v>17</v>
+      </c>
+      <c r="E308">
+        <v>122.24166666666669</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12091,10 +12292,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F295"/>
+  <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView topLeftCell="A253" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E283" sqref="E283:E295"/>
+    <sheetView topLeftCell="A265" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E296" sqref="E296:E308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -17364,6 +17565,227 @@
         <v>115.55833333333334</v>
       </c>
     </row>
+    <row r="296" spans="1:5">
+      <c r="A296" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C296" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E296">
+        <v>120.75833333333333</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" t="s">
+        <v>6</v>
+      </c>
+      <c r="B297" t="s">
+        <v>30</v>
+      </c>
+      <c r="C297">
+        <v>2023</v>
+      </c>
+      <c r="D297" t="s">
+        <v>18</v>
+      </c>
+      <c r="E297">
+        <v>135.55833333333337</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" t="s">
+        <v>6</v>
+      </c>
+      <c r="B298" t="s">
+        <v>30</v>
+      </c>
+      <c r="C298">
+        <v>2023</v>
+      </c>
+      <c r="D298" t="s">
+        <v>19</v>
+      </c>
+      <c r="E298">
+        <v>173.35833333333335</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" t="s">
+        <v>6</v>
+      </c>
+      <c r="B299" t="s">
+        <v>30</v>
+      </c>
+      <c r="C299">
+        <v>2023</v>
+      </c>
+      <c r="D299" t="s">
+        <v>20</v>
+      </c>
+      <c r="E299">
+        <v>91.008333333333326</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" t="s">
+        <v>6</v>
+      </c>
+      <c r="B300" t="s">
+        <v>30</v>
+      </c>
+      <c r="C300">
+        <v>2023</v>
+      </c>
+      <c r="D300" t="s">
+        <v>21</v>
+      </c>
+      <c r="E300">
+        <v>111.67500000000003</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" t="s">
+        <v>6</v>
+      </c>
+      <c r="B301" t="s">
+        <v>30</v>
+      </c>
+      <c r="C301">
+        <v>2023</v>
+      </c>
+      <c r="D301" t="s">
+        <v>22</v>
+      </c>
+      <c r="E301">
+        <v>117.83333333333333</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" t="s">
+        <v>6</v>
+      </c>
+      <c r="B302" t="s">
+        <v>30</v>
+      </c>
+      <c r="C302">
+        <v>2023</v>
+      </c>
+      <c r="D302" t="s">
+        <v>23</v>
+      </c>
+      <c r="E302">
+        <v>132.39166666666668</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" t="s">
+        <v>6</v>
+      </c>
+      <c r="B303" t="s">
+        <v>30</v>
+      </c>
+      <c r="C303">
+        <v>2023</v>
+      </c>
+      <c r="D303" t="s">
+        <v>24</v>
+      </c>
+      <c r="E303">
+        <v>114.22500000000001</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" t="s">
+        <v>6</v>
+      </c>
+      <c r="B304" t="s">
+        <v>30</v>
+      </c>
+      <c r="C304">
+        <v>2023</v>
+      </c>
+      <c r="D304" t="s">
+        <v>25</v>
+      </c>
+      <c r="E304">
+        <v>97.866666666666674</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" t="s">
+        <v>6</v>
+      </c>
+      <c r="B305" t="s">
+        <v>30</v>
+      </c>
+      <c r="C305">
+        <v>2023</v>
+      </c>
+      <c r="D305" t="s">
+        <v>26</v>
+      </c>
+      <c r="E305">
+        <v>120.49166666666666</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" t="s">
+        <v>6</v>
+      </c>
+      <c r="B306" t="s">
+        <v>30</v>
+      </c>
+      <c r="C306">
+        <v>2023</v>
+      </c>
+      <c r="D306" t="s">
+        <v>27</v>
+      </c>
+      <c r="E306">
+        <v>116.30833333333335</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" t="s">
+        <v>6</v>
+      </c>
+      <c r="B307" t="s">
+        <v>30</v>
+      </c>
+      <c r="C307">
+        <v>2023</v>
+      </c>
+      <c r="D307" t="s">
+        <v>28</v>
+      </c>
+      <c r="E307">
+        <v>153.50833333333333</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" t="s">
+        <v>6</v>
+      </c>
+      <c r="B308" t="s">
+        <v>30</v>
+      </c>
+      <c r="C308">
+        <v>2023</v>
+      </c>
+      <c r="D308" t="s">
+        <v>17</v>
+      </c>
+      <c r="E308">
+        <v>118.64999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -17372,10 +17794,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AC295"/>
+  <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView topLeftCell="A253" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E283" sqref="E283:E295"/>
+    <sheetView topLeftCell="A262" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E296" sqref="E296:E308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -21982,7 +22404,7 @@
         <v>111.4</v>
       </c>
     </row>
-    <row r="257" spans="1:29">
+    <row r="257" spans="1:5">
       <c r="A257" s="3" t="s">
         <v>6</v>
       </c>
@@ -21999,7 +22421,7 @@
         <v>114.7</v>
       </c>
     </row>
-    <row r="258" spans="1:29">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>6</v>
       </c>
@@ -22016,7 +22438,7 @@
         <v>128.5</v>
       </c>
     </row>
-    <row r="259" spans="1:29">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>6</v>
       </c>
@@ -22033,7 +22455,7 @@
         <v>146.9</v>
       </c>
     </row>
-    <row r="260" spans="1:29">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>6</v>
       </c>
@@ -22050,7 +22472,7 @@
         <v>90.2</v>
       </c>
     </row>
-    <row r="261" spans="1:29">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>6</v>
       </c>
@@ -22067,7 +22489,7 @@
         <v>109.2</v>
       </c>
     </row>
-    <row r="262" spans="1:29">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>6</v>
       </c>
@@ -22084,7 +22506,7 @@
         <v>107.9</v>
       </c>
     </row>
-    <row r="263" spans="1:29">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
         <v>6</v>
       </c>
@@ -22101,7 +22523,7 @@
         <v>128.9</v>
       </c>
     </row>
-    <row r="264" spans="1:29">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>6</v>
       </c>
@@ -22118,7 +22540,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="265" spans="1:29">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>6</v>
       </c>
@@ -22135,7 +22557,7 @@
         <v>95.9</v>
       </c>
     </row>
-    <row r="266" spans="1:29">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
         <v>6</v>
       </c>
@@ -22152,7 +22574,7 @@
         <v>104.4</v>
       </c>
     </row>
-    <row r="267" spans="1:29">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
         <v>6</v>
       </c>
@@ -22169,7 +22591,7 @@
         <v>114.4</v>
       </c>
     </row>
-    <row r="268" spans="1:29">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>6</v>
       </c>
@@ -22186,7 +22608,7 @@
         <v>127.3</v>
       </c>
     </row>
-    <row r="269" spans="1:29">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
         <v>6</v>
       </c>
@@ -22203,7 +22625,7 @@
         <v>114.2</v>
       </c>
     </row>
-    <row r="270" spans="1:29">
+    <row r="270" spans="1:5">
       <c r="A270" s="3" t="s">
         <v>6</v>
       </c>
@@ -22220,7 +22642,7 @@
         <v>117.112378890683</v>
       </c>
     </row>
-    <row r="271" spans="1:29">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>6</v>
       </c>
@@ -22236,47 +22658,8 @@
       <c r="E271" s="4">
         <v>129.98830743860501</v>
       </c>
-      <c r="Q271">
-        <v>120.79166666666667</v>
-      </c>
-      <c r="R271">
-        <v>137.08333333333334</v>
-      </c>
-      <c r="S271">
-        <v>147.55000000000004</v>
-      </c>
-      <c r="T271">
-        <v>89.758333333333326</v>
-      </c>
-      <c r="U271">
-        <v>109.68333333333334</v>
-      </c>
-      <c r="V271">
-        <v>111.44166666666666</v>
-      </c>
-      <c r="W271">
-        <v>128.18333333333331</v>
-      </c>
-      <c r="X271">
-        <v>122.22499999999998</v>
-      </c>
-      <c r="Y271">
-        <v>95.899999999999991</v>
-      </c>
-      <c r="Z271">
-        <v>107.77499999999999</v>
-      </c>
-      <c r="AA271">
-        <v>115.33333333333336</v>
-      </c>
-      <c r="AB271">
-        <v>134.78333333333333</v>
-      </c>
-      <c r="AC271">
-        <v>116.17500000000001</v>
-      </c>
-    </row>
-    <row r="272" spans="1:29">
+    </row>
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
         <v>6</v>
       </c>
@@ -22293,7 +22676,7 @@
         <v>147.390328096232</v>
       </c>
     </row>
-    <row r="273" spans="1:17">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>6</v>
       </c>
@@ -22309,11 +22692,8 @@
       <c r="E273" s="4">
         <v>89.809741762490205</v>
       </c>
-      <c r="Q273">
-        <v>120.79166666666667</v>
-      </c>
-    </row>
-    <row r="274" spans="1:17">
+    </row>
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>6</v>
       </c>
@@ -22329,11 +22709,8 @@
       <c r="E274" s="4">
         <v>108.725642949617</v>
       </c>
-      <c r="Q274">
-        <v>137.08333333333334</v>
-      </c>
-    </row>
-    <row r="275" spans="1:17">
+    </row>
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>6</v>
       </c>
@@ -22349,11 +22726,8 @@
       <c r="E275" s="4">
         <v>108.899144800364</v>
       </c>
-      <c r="Q275">
-        <v>147.55000000000004</v>
-      </c>
-    </row>
-    <row r="276" spans="1:17">
+    </row>
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>6</v>
       </c>
@@ -22369,11 +22743,8 @@
       <c r="E276" s="4">
         <v>129.10098893821799</v>
       </c>
-      <c r="Q276">
-        <v>89.758333333333326</v>
-      </c>
-    </row>
-    <row r="277" spans="1:17">
+    </row>
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>6</v>
       </c>
@@ -22389,11 +22760,8 @@
       <c r="E277" s="4">
         <v>117.573897290712</v>
       </c>
-      <c r="Q277">
-        <v>109.68333333333334</v>
-      </c>
-    </row>
-    <row r="278" spans="1:17">
+    </row>
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>6</v>
       </c>
@@ -22409,11 +22777,8 @@
       <c r="E278" s="4">
         <v>95.907911749999997</v>
       </c>
-      <c r="Q278">
-        <v>111.44166666666666</v>
-      </c>
-    </row>
-    <row r="279" spans="1:17">
+    </row>
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>6</v>
       </c>
@@ -22429,11 +22794,8 @@
       <c r="E279" s="4">
         <v>102.827606866731</v>
       </c>
-      <c r="Q279">
-        <v>128.18333333333331</v>
-      </c>
-    </row>
-    <row r="280" spans="1:17">
+    </row>
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>6</v>
       </c>
@@ -22449,11 +22811,8 @@
       <c r="E280" s="4">
         <v>113.617128206733</v>
       </c>
-      <c r="Q280">
-        <v>122.22499999999998</v>
-      </c>
-    </row>
-    <row r="281" spans="1:17">
+    </row>
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>6</v>
       </c>
@@ -22469,11 +22828,8 @@
       <c r="E281" s="4">
         <v>128.299504907657</v>
       </c>
-      <c r="Q281">
-        <v>95.899999999999991</v>
-      </c>
-    </row>
-    <row r="282" spans="1:17">
+    </row>
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>6</v>
       </c>
@@ -22489,11 +22845,8 @@
       <c r="E282" s="4">
         <v>114.850271827345</v>
       </c>
-      <c r="Q282">
-        <v>107.77499999999999</v>
-      </c>
-    </row>
-    <row r="283" spans="1:17">
+    </row>
+    <row r="283" spans="1:5">
       <c r="A283" s="3" t="s">
         <v>6</v>
       </c>
@@ -22509,11 +22862,8 @@
       <c r="E283">
         <v>120.79166666666667</v>
       </c>
-      <c r="Q283">
-        <v>115.33333333333336</v>
-      </c>
-    </row>
-    <row r="284" spans="1:17">
+    </row>
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
         <v>6</v>
       </c>
@@ -22529,11 +22879,8 @@
       <c r="E284">
         <v>137.08333333333334</v>
       </c>
-      <c r="Q284">
-        <v>134.78333333333333</v>
-      </c>
-    </row>
-    <row r="285" spans="1:17">
+    </row>
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>6</v>
       </c>
@@ -22549,11 +22896,8 @@
       <c r="E285">
         <v>147.55000000000004</v>
       </c>
-      <c r="Q285">
-        <v>116.17500000000001</v>
-      </c>
-    </row>
-    <row r="286" spans="1:17">
+    </row>
+    <row r="286" spans="1:5">
       <c r="A286" t="s">
         <v>6</v>
       </c>
@@ -22570,7 +22914,7 @@
         <v>89.758333333333326</v>
       </c>
     </row>
-    <row r="287" spans="1:17">
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
         <v>6</v>
       </c>
@@ -22587,7 +22931,7 @@
         <v>109.68333333333334</v>
       </c>
     </row>
-    <row r="288" spans="1:17">
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>6</v>
       </c>
@@ -22721,6 +23065,227 @@
       </c>
       <c r="E295">
         <v>116.17500000000001</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5">
+      <c r="A296" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C296" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E296">
+        <v>124.51666666666667</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" t="s">
+        <v>6</v>
+      </c>
+      <c r="B297" t="s">
+        <v>31</v>
+      </c>
+      <c r="C297">
+        <v>2023</v>
+      </c>
+      <c r="D297" t="s">
+        <v>18</v>
+      </c>
+      <c r="E297">
+        <v>145.45833333333334</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" t="s">
+        <v>6</v>
+      </c>
+      <c r="B298" t="s">
+        <v>31</v>
+      </c>
+      <c r="C298">
+        <v>2023</v>
+      </c>
+      <c r="D298" t="s">
+        <v>19</v>
+      </c>
+      <c r="E298">
+        <v>148.85833333333335</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" t="s">
+        <v>6</v>
+      </c>
+      <c r="B299" t="s">
+        <v>31</v>
+      </c>
+      <c r="C299">
+        <v>2023</v>
+      </c>
+      <c r="D299" t="s">
+        <v>20</v>
+      </c>
+      <c r="E299">
+        <v>90.016666666666666</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" t="s">
+        <v>6</v>
+      </c>
+      <c r="B300" t="s">
+        <v>31</v>
+      </c>
+      <c r="C300">
+        <v>2023</v>
+      </c>
+      <c r="D300" t="s">
+        <v>21</v>
+      </c>
+      <c r="E300">
+        <v>111.68333333333332</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" t="s">
+        <v>6</v>
+      </c>
+      <c r="B301" t="s">
+        <v>31</v>
+      </c>
+      <c r="C301">
+        <v>2023</v>
+      </c>
+      <c r="D301" t="s">
+        <v>22</v>
+      </c>
+      <c r="E301">
+        <v>114.05833333333332</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" t="s">
+        <v>6</v>
+      </c>
+      <c r="B302" t="s">
+        <v>31</v>
+      </c>
+      <c r="C302">
+        <v>2023</v>
+      </c>
+      <c r="D302" t="s">
+        <v>23</v>
+      </c>
+      <c r="E302">
+        <v>130.30833333333337</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" t="s">
+        <v>6</v>
+      </c>
+      <c r="B303" t="s">
+        <v>31</v>
+      </c>
+      <c r="C303">
+        <v>2023</v>
+      </c>
+      <c r="D303" t="s">
+        <v>24</v>
+      </c>
+      <c r="E303">
+        <v>123.06666666666668</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" t="s">
+        <v>6</v>
+      </c>
+      <c r="B304" t="s">
+        <v>31</v>
+      </c>
+      <c r="C304">
+        <v>2023</v>
+      </c>
+      <c r="D304" t="s">
+        <v>25</v>
+      </c>
+      <c r="E304">
+        <v>94.366666666666674</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" t="s">
+        <v>6</v>
+      </c>
+      <c r="B305" t="s">
+        <v>31</v>
+      </c>
+      <c r="C305">
+        <v>2023</v>
+      </c>
+      <c r="D305" t="s">
+        <v>26</v>
+      </c>
+      <c r="E305">
+        <v>108.3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" t="s">
+        <v>6</v>
+      </c>
+      <c r="B306" t="s">
+        <v>31</v>
+      </c>
+      <c r="C306">
+        <v>2023</v>
+      </c>
+      <c r="D306" t="s">
+        <v>27</v>
+      </c>
+      <c r="E306">
+        <v>118.11666666666667</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" t="s">
+        <v>6</v>
+      </c>
+      <c r="B307" t="s">
+        <v>31</v>
+      </c>
+      <c r="C307">
+        <v>2023</v>
+      </c>
+      <c r="D307" t="s">
+        <v>28</v>
+      </c>
+      <c r="E307">
+        <v>141.93333333333331</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" t="s">
+        <v>6</v>
+      </c>
+      <c r="B308" t="s">
+        <v>31</v>
+      </c>
+      <c r="C308">
+        <v>2023</v>
+      </c>
+      <c r="D308" t="s">
+        <v>17</v>
+      </c>
+      <c r="E308">
+        <v>119.13333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -22731,11 +23296,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:AF295"/>
+  <dimension ref="B1:AF308"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD289" sqref="AD289"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z296" sqref="Z296:AF308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -39020,7 +39585,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="289" spans="4:32">
+    <row r="289" spans="2:32">
       <c r="D289" t="s">
         <v>43</v>
       </c>
@@ -39070,7 +39635,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="290" spans="4:32">
+    <row r="290" spans="2:32">
       <c r="D290" t="s">
         <v>44</v>
       </c>
@@ -39120,7 +39685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="291" spans="4:32">
+    <row r="291" spans="2:32">
       <c r="D291" t="s">
         <v>45</v>
       </c>
@@ -39170,7 +39735,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="292" spans="4:32">
+    <row r="292" spans="2:32">
       <c r="D292" t="s">
         <v>46</v>
       </c>
@@ -39220,7 +39785,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="293" spans="4:32">
+    <row r="293" spans="2:32">
       <c r="D293" t="s">
         <v>47</v>
       </c>
@@ -39270,7 +39835,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="294" spans="4:32">
+    <row r="294" spans="2:32">
       <c r="D294" t="s">
         <v>50</v>
       </c>
@@ -39320,7 +39885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="295" spans="4:32">
+    <row r="295" spans="2:32">
       <c r="D295" t="s">
         <v>48</v>
       </c>
@@ -39382,9 +39947,695 @@
         <v>49</v>
       </c>
     </row>
+    <row r="296" spans="2:32">
+      <c r="B296">
+        <v>2023</v>
+      </c>
+      <c r="C296" t="s">
+        <v>34</v>
+      </c>
+      <c r="D296" t="s">
+        <v>35</v>
+      </c>
+      <c r="E296" t="s">
+        <v>36</v>
+      </c>
+      <c r="F296">
+        <v>130.37500000000003</v>
+      </c>
+      <c r="G296" t="s">
+        <v>37</v>
+      </c>
+      <c r="J296">
+        <v>2023</v>
+      </c>
+      <c r="K296" t="s">
+        <v>34</v>
+      </c>
+      <c r="L296" t="s">
+        <v>35</v>
+      </c>
+      <c r="M296" t="s">
+        <v>36</v>
+      </c>
+      <c r="N296">
+        <v>131.65833333333333</v>
+      </c>
+      <c r="O296" t="s">
+        <v>37</v>
+      </c>
+      <c r="R296">
+        <v>2023</v>
+      </c>
+      <c r="S296" t="s">
+        <v>34</v>
+      </c>
+      <c r="T296" t="s">
+        <v>35</v>
+      </c>
+      <c r="U296" t="s">
+        <v>36</v>
+      </c>
+      <c r="V296">
+        <v>120.75833333333333</v>
+      </c>
+      <c r="W296" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z296">
+        <v>2023</v>
+      </c>
+      <c r="AA296" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB296" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC296" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD296">
+        <v>124.51666666666667</v>
+      </c>
+      <c r="AE296" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="297" spans="2:32">
+      <c r="D297" t="s">
+        <v>38</v>
+      </c>
+      <c r="E297" t="s">
+        <v>36</v>
+      </c>
+      <c r="F297">
+        <v>151.98333333333329</v>
+      </c>
+      <c r="G297" t="s">
+        <v>37</v>
+      </c>
+      <c r="L297" t="s">
+        <v>38</v>
+      </c>
+      <c r="M297" t="s">
+        <v>36</v>
+      </c>
+      <c r="N297">
+        <v>154.13333333333333</v>
+      </c>
+      <c r="O297" t="s">
+        <v>37</v>
+      </c>
+      <c r="T297" t="s">
+        <v>38</v>
+      </c>
+      <c r="U297" t="s">
+        <v>36</v>
+      </c>
+      <c r="V297">
+        <v>135.55833333333337</v>
+      </c>
+      <c r="W297" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB297" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC297" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD297">
+        <v>145.45833333333334</v>
+      </c>
+      <c r="AE297" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="298" spans="2:32">
+      <c r="D298" t="s">
+        <v>39</v>
+      </c>
+      <c r="E298" t="s">
+        <v>36</v>
+      </c>
+      <c r="F298">
+        <v>171.24166666666667</v>
+      </c>
+      <c r="G298" t="s">
+        <v>37</v>
+      </c>
+      <c r="L298" t="s">
+        <v>39</v>
+      </c>
+      <c r="M298" t="s">
+        <v>36</v>
+      </c>
+      <c r="N298">
+        <v>173.04166666666666</v>
+      </c>
+      <c r="O298" t="s">
+        <v>37</v>
+      </c>
+      <c r="T298" t="s">
+        <v>39</v>
+      </c>
+      <c r="U298" t="s">
+        <v>36</v>
+      </c>
+      <c r="V298">
+        <v>173.35833333333335</v>
+      </c>
+      <c r="W298" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB298" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC298" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD298">
+        <v>148.85833333333335</v>
+      </c>
+      <c r="AE298" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="299" spans="2:32">
+      <c r="D299" t="s">
+        <v>40</v>
+      </c>
+      <c r="E299" t="s">
+        <v>36</v>
+      </c>
+      <c r="F299">
+        <v>93.458333333333329</v>
+      </c>
+      <c r="G299" t="s">
+        <v>37</v>
+      </c>
+      <c r="L299" t="s">
+        <v>40</v>
+      </c>
+      <c r="M299" t="s">
+        <v>36</v>
+      </c>
+      <c r="N299">
+        <v>93.916666666666671</v>
+      </c>
+      <c r="O299" t="s">
+        <v>37</v>
+      </c>
+      <c r="T299" t="s">
+        <v>40</v>
+      </c>
+      <c r="U299" t="s">
+        <v>36</v>
+      </c>
+      <c r="V299">
+        <v>91.008333333333326</v>
+      </c>
+      <c r="W299" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB299" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC299" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD299">
+        <v>90.016666666666666</v>
+      </c>
+      <c r="AE299" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="300" spans="2:32">
+      <c r="D300" t="s">
+        <v>41</v>
+      </c>
+      <c r="E300" t="s">
+        <v>36</v>
+      </c>
+      <c r="F300">
+        <v>125.25833333333333</v>
+      </c>
+      <c r="G300" t="s">
+        <v>37</v>
+      </c>
+      <c r="L300" t="s">
+        <v>41</v>
+      </c>
+      <c r="M300" t="s">
+        <v>36</v>
+      </c>
+      <c r="N300">
+        <v>127.71666666666668</v>
+      </c>
+      <c r="O300" t="s">
+        <v>37</v>
+      </c>
+      <c r="T300" t="s">
+        <v>41</v>
+      </c>
+      <c r="U300" t="s">
+        <v>36</v>
+      </c>
+      <c r="V300">
+        <v>111.67500000000003</v>
+      </c>
+      <c r="W300" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB300" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC300" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD300">
+        <v>111.68333333333332</v>
+      </c>
+      <c r="AE300" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="301" spans="2:32">
+      <c r="D301" t="s">
+        <v>42</v>
+      </c>
+      <c r="E301" t="s">
+        <v>36</v>
+      </c>
+      <c r="F301">
+        <v>125.60833333333333</v>
+      </c>
+      <c r="G301" t="s">
+        <v>37</v>
+      </c>
+      <c r="L301" t="s">
+        <v>42</v>
+      </c>
+      <c r="M301" t="s">
+        <v>36</v>
+      </c>
+      <c r="N301">
+        <v>127.24166666666667</v>
+      </c>
+      <c r="O301" t="s">
+        <v>37</v>
+      </c>
+      <c r="T301" t="s">
+        <v>42</v>
+      </c>
+      <c r="U301" t="s">
+        <v>36</v>
+      </c>
+      <c r="V301">
+        <v>117.83333333333333</v>
+      </c>
+      <c r="W301" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB301" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC301" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD301">
+        <v>114.05833333333332</v>
+      </c>
+      <c r="AE301" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="302" spans="2:32">
+      <c r="D302" t="s">
+        <v>43</v>
+      </c>
+      <c r="E302" t="s">
+        <v>36</v>
+      </c>
+      <c r="F302">
+        <v>128.16666666666666</v>
+      </c>
+      <c r="G302" t="s">
+        <v>37</v>
+      </c>
+      <c r="L302" t="s">
+        <v>43</v>
+      </c>
+      <c r="M302" t="s">
+        <v>36</v>
+      </c>
+      <c r="N302">
+        <v>127.74166666666666</v>
+      </c>
+      <c r="O302" t="s">
+        <v>37</v>
+      </c>
+      <c r="T302" t="s">
+        <v>43</v>
+      </c>
+      <c r="U302" t="s">
+        <v>36</v>
+      </c>
+      <c r="V302">
+        <v>132.39166666666668</v>
+      </c>
+      <c r="W302" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB302" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC302" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD302">
+        <v>130.30833333333337</v>
+      </c>
+      <c r="AE302" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="303" spans="2:32">
+      <c r="D303" t="s">
+        <v>44</v>
+      </c>
+      <c r="E303" t="s">
+        <v>36</v>
+      </c>
+      <c r="F303">
+        <v>120.50000000000001</v>
+      </c>
+      <c r="G303" t="s">
+        <v>37</v>
+      </c>
+      <c r="L303" t="s">
+        <v>44</v>
+      </c>
+      <c r="M303" t="s">
+        <v>36</v>
+      </c>
+      <c r="N303">
+        <v>120.68333333333334</v>
+      </c>
+      <c r="O303" t="s">
+        <v>37</v>
+      </c>
+      <c r="T303" t="s">
+        <v>44</v>
+      </c>
+      <c r="U303" t="s">
+        <v>36</v>
+      </c>
+      <c r="V303">
+        <v>114.22500000000001</v>
+      </c>
+      <c r="W303" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB303" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC303" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD303">
+        <v>123.06666666666668</v>
+      </c>
+      <c r="AE303" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="304" spans="2:32">
+      <c r="D304" t="s">
+        <v>45</v>
+      </c>
+      <c r="E304" t="s">
+        <v>36</v>
+      </c>
+      <c r="F304">
+        <v>94.641666666666666</v>
+      </c>
+      <c r="G304" t="s">
+        <v>37</v>
+      </c>
+      <c r="L304" t="s">
+        <v>45</v>
+      </c>
+      <c r="M304" t="s">
+        <v>36</v>
+      </c>
+      <c r="N304">
+        <v>94.441666666666677</v>
+      </c>
+      <c r="O304" t="s">
+        <v>37</v>
+      </c>
+      <c r="T304" t="s">
+        <v>45</v>
+      </c>
+      <c r="U304" t="s">
+        <v>36</v>
+      </c>
+      <c r="V304">
+        <v>97.866666666666674</v>
+      </c>
+      <c r="W304" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB304" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC304" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD304">
+        <v>94.366666666666674</v>
+      </c>
+      <c r="AE304" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="305" spans="4:32">
+      <c r="D305" t="s">
+        <v>46</v>
+      </c>
+      <c r="E305" t="s">
+        <v>36</v>
+      </c>
+      <c r="F305">
+        <v>117.00833333333333</v>
+      </c>
+      <c r="G305" t="s">
+        <v>37</v>
+      </c>
+      <c r="L305" t="s">
+        <v>46</v>
+      </c>
+      <c r="M305" t="s">
+        <v>36</v>
+      </c>
+      <c r="N305">
+        <v>117.44166666666666</v>
+      </c>
+      <c r="O305" t="s">
+        <v>37</v>
+      </c>
+      <c r="T305" t="s">
+        <v>46</v>
+      </c>
+      <c r="U305" t="s">
+        <v>36</v>
+      </c>
+      <c r="V305">
+        <v>120.49166666666666</v>
+      </c>
+      <c r="W305" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB305" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC305" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD305">
+        <v>108.3</v>
+      </c>
+      <c r="AE305" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="306" spans="4:32">
+      <c r="D306" t="s">
+        <v>47</v>
+      </c>
+      <c r="E306" t="s">
+        <v>36</v>
+      </c>
+      <c r="F306">
+        <v>124.66666666666664</v>
+      </c>
+      <c r="G306" t="s">
+        <v>37</v>
+      </c>
+      <c r="L306" t="s">
+        <v>47</v>
+      </c>
+      <c r="M306" t="s">
+        <v>36</v>
+      </c>
+      <c r="N306">
+        <v>125.51666666666667</v>
+      </c>
+      <c r="O306" t="s">
+        <v>37</v>
+      </c>
+      <c r="T306" t="s">
+        <v>47</v>
+      </c>
+      <c r="U306" t="s">
+        <v>36</v>
+      </c>
+      <c r="V306">
+        <v>116.30833333333335</v>
+      </c>
+      <c r="W306" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB306" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC306" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD306">
+        <v>118.11666666666667</v>
+      </c>
+      <c r="AE306" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="307" spans="4:32">
+      <c r="D307" t="s">
+        <v>50</v>
+      </c>
+      <c r="E307" t="s">
+        <v>36</v>
+      </c>
+      <c r="F307">
+        <v>147.24999999999997</v>
+      </c>
+      <c r="G307" t="s">
+        <v>37</v>
+      </c>
+      <c r="L307" t="s">
+        <v>50</v>
+      </c>
+      <c r="M307" t="s">
+        <v>36</v>
+      </c>
+      <c r="N307">
+        <v>147.30833333333334</v>
+      </c>
+      <c r="O307" t="s">
+        <v>37</v>
+      </c>
+      <c r="T307" t="s">
+        <v>50</v>
+      </c>
+      <c r="U307" t="s">
+        <v>36</v>
+      </c>
+      <c r="V307">
+        <v>153.50833333333333</v>
+      </c>
+      <c r="W307" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB307" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC307" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD307">
+        <v>141.93333333333331</v>
+      </c>
+      <c r="AE307" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="308" spans="4:32">
+      <c r="D308" t="s">
+        <v>48</v>
+      </c>
+      <c r="E308" t="s">
+        <v>36</v>
+      </c>
+      <c r="F308">
+        <v>121.78333333333332</v>
+      </c>
+      <c r="G308" t="s">
+        <v>37</v>
+      </c>
+      <c r="H308" t="s">
+        <v>49</v>
+      </c>
+      <c r="L308" t="s">
+        <v>48</v>
+      </c>
+      <c r="M308" t="s">
+        <v>36</v>
+      </c>
+      <c r="N308">
+        <v>122.24166666666669</v>
+      </c>
+      <c r="O308" t="s">
+        <v>37</v>
+      </c>
+      <c r="P308" t="s">
+        <v>49</v>
+      </c>
+      <c r="T308" t="s">
+        <v>48</v>
+      </c>
+      <c r="U308" t="s">
+        <v>36</v>
+      </c>
+      <c r="V308">
+        <v>118.64999999999998</v>
+      </c>
+      <c r="W308" t="s">
+        <v>37</v>
+      </c>
+      <c r="X308" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB308" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC308" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD308">
+        <v>119.13333333333333</v>
+      </c>
+      <c r="AE308" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF308" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Deploying to gh-pages from @ xkre/malaysia-inflation-calc@15a5865d6226efa505c4594f860a0d0bf4b6493c 🚀
</commit_message>
<xml_diff>
--- a/data/CpiDataset.xlsx
+++ b/data/CpiDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arekr\source\repos\malaysia-inflation-calc\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8891B665-D26A-4819-9C97-4D8C809E1069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E9C383-CBF8-4CED-8F53-ECB393F122DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Malaysia" sheetId="1" r:id="rId1"/>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E296" sqref="E296:E308"/>
     </sheetView>
   </sheetViews>
@@ -6575,7 +6575,7 @@
         <v>8</v>
       </c>
       <c r="E296">
-        <v>130.37500000000003</v>
+        <v>130.4</v>
       </c>
     </row>
     <row r="297" spans="1:5">
@@ -6592,7 +6592,7 @@
         <v>18</v>
       </c>
       <c r="E297">
-        <v>151.98333333333329</v>
+        <v>152.01666666666662</v>
       </c>
     </row>
     <row r="298" spans="1:5">
@@ -6609,7 +6609,7 @@
         <v>19</v>
       </c>
       <c r="E298">
-        <v>171.24166666666667</v>
+        <v>171.22499999999999</v>
       </c>
     </row>
     <row r="299" spans="1:5">
@@ -6677,7 +6677,7 @@
         <v>23</v>
       </c>
       <c r="E302">
-        <v>128.16666666666666</v>
+        <v>128.18333333333331</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -6694,7 +6694,7 @@
         <v>24</v>
       </c>
       <c r="E303">
-        <v>120.50000000000001</v>
+        <v>120.53333333333335</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -6711,7 +6711,7 @@
         <v>25</v>
       </c>
       <c r="E304">
-        <v>94.641666666666666</v>
+        <v>94.633333333333326</v>
       </c>
     </row>
     <row r="305" spans="1:5">
@@ -6728,7 +6728,7 @@
         <v>26</v>
       </c>
       <c r="E305">
-        <v>117.00833333333333</v>
+        <v>117.05</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -6762,7 +6762,7 @@
         <v>28</v>
       </c>
       <c r="E307">
-        <v>147.24999999999997</v>
+        <v>147.26666666666665</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -6779,7 +6779,7 @@
         <v>17</v>
       </c>
       <c r="E308">
-        <v>121.78333333333332</v>
+        <v>121.80833333333332</v>
       </c>
     </row>
   </sheetData>
@@ -6792,8 +6792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S276" sqref="S276"/>
+    <sheetView topLeftCell="A262" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E296" sqref="E296:E308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -12077,7 +12077,7 @@
         <v>8</v>
       </c>
       <c r="E296">
-        <v>131.65833333333333</v>
+        <v>131.67499999999998</v>
       </c>
     </row>
     <row r="297" spans="1:5">
@@ -12094,7 +12094,7 @@
         <v>18</v>
       </c>
       <c r="E297">
-        <v>154.13333333333333</v>
+        <v>154.17499999999998</v>
       </c>
     </row>
     <row r="298" spans="1:5">
@@ -12111,7 +12111,7 @@
         <v>19</v>
       </c>
       <c r="E298">
-        <v>173.04166666666666</v>
+        <v>173.02499999999998</v>
       </c>
     </row>
     <row r="299" spans="1:5">
@@ -12179,7 +12179,7 @@
         <v>23</v>
       </c>
       <c r="E302">
-        <v>127.74166666666666</v>
+        <v>127.75833333333333</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -12196,7 +12196,7 @@
         <v>24</v>
       </c>
       <c r="E303">
-        <v>120.68333333333334</v>
+        <v>120.71666666666668</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -12213,7 +12213,7 @@
         <v>25</v>
       </c>
       <c r="E304">
-        <v>94.441666666666677</v>
+        <v>94.433333333333337</v>
       </c>
     </row>
     <row r="305" spans="1:5">
@@ -12230,7 +12230,7 @@
         <v>26</v>
       </c>
       <c r="E305">
-        <v>117.44166666666666</v>
+        <v>117.47500000000001</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -12264,7 +12264,7 @@
         <v>28</v>
       </c>
       <c r="E307">
-        <v>147.30833333333334</v>
+        <v>147.33333333333334</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -12281,7 +12281,7 @@
         <v>17</v>
       </c>
       <c r="E308">
-        <v>122.24166666666669</v>
+        <v>122.27500000000002</v>
       </c>
     </row>
   </sheetData>
@@ -12292,7 +12292,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F308"/>
+  <dimension ref="A1:R308"/>
   <sheetViews>
     <sheetView topLeftCell="A265" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E296" sqref="E296:E308"/>
@@ -12305,6 +12305,7 @@
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="67.81640625" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17446,7 +17447,7 @@
         <v>115.45833333333331</v>
       </c>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:18">
       <c r="A289" t="s">
         <v>6</v>
       </c>
@@ -17463,7 +17464,7 @@
         <v>130.75</v>
       </c>
     </row>
-    <row r="290" spans="1:5">
+    <row r="290" spans="1:18">
       <c r="A290" t="s">
         <v>6</v>
       </c>
@@ -17480,7 +17481,7 @@
         <v>114.29166666666664</v>
       </c>
     </row>
-    <row r="291" spans="1:5">
+    <row r="291" spans="1:18">
       <c r="A291" t="s">
         <v>6</v>
       </c>
@@ -17496,8 +17497,9 @@
       <c r="E291">
         <v>99.183333333333337</v>
       </c>
-    </row>
-    <row r="292" spans="1:5">
+      <c r="R291" s="12"/>
+    </row>
+    <row r="292" spans="1:18">
       <c r="A292" t="s">
         <v>6</v>
       </c>
@@ -17513,8 +17515,9 @@
       <c r="E292">
         <v>119.47499999999998</v>
       </c>
-    </row>
-    <row r="293" spans="1:5">
+      <c r="R292" s="12"/>
+    </row>
+    <row r="293" spans="1:18">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -17530,8 +17533,9 @@
       <c r="E293">
         <v>114.41666666666667</v>
       </c>
-    </row>
-    <row r="294" spans="1:5">
+      <c r="R293" s="12"/>
+    </row>
+    <row r="294" spans="1:18">
       <c r="A294" t="s">
         <v>6</v>
       </c>
@@ -17547,8 +17551,9 @@
       <c r="E294">
         <v>145.50833333333335</v>
       </c>
-    </row>
-    <row r="295" spans="1:5">
+      <c r="R294" s="12"/>
+    </row>
+    <row r="295" spans="1:18">
       <c r="A295" t="s">
         <v>6</v>
       </c>
@@ -17564,8 +17569,9 @@
       <c r="E295">
         <v>115.55833333333334</v>
       </c>
-    </row>
-    <row r="296" spans="1:5">
+      <c r="R295" s="12"/>
+    </row>
+    <row r="296" spans="1:18">
       <c r="A296" s="3" t="s">
         <v>6</v>
       </c>
@@ -17579,10 +17585,11 @@
         <v>8</v>
       </c>
       <c r="E296">
-        <v>120.75833333333333</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5">
+        <v>120.76666666666667</v>
+      </c>
+      <c r="R296" s="12"/>
+    </row>
+    <row r="297" spans="1:18">
       <c r="A297" t="s">
         <v>6</v>
       </c>
@@ -17596,10 +17603,11 @@
         <v>18</v>
       </c>
       <c r="E297">
-        <v>135.55833333333337</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5">
+        <v>135.56666666666669</v>
+      </c>
+      <c r="R297" s="12"/>
+    </row>
+    <row r="298" spans="1:18">
       <c r="A298" t="s">
         <v>6</v>
       </c>
@@ -17613,10 +17621,11 @@
         <v>19</v>
       </c>
       <c r="E298">
-        <v>173.35833333333335</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5">
+        <v>173.36666666666667</v>
+      </c>
+      <c r="R298" s="12"/>
+    </row>
+    <row r="299" spans="1:18">
       <c r="A299" t="s">
         <v>6</v>
       </c>
@@ -17630,10 +17639,11 @@
         <v>20</v>
       </c>
       <c r="E299">
-        <v>91.008333333333326</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5">
+        <v>90.999999999999986</v>
+      </c>
+      <c r="R299" s="12"/>
+    </row>
+    <row r="300" spans="1:18">
       <c r="A300" t="s">
         <v>6</v>
       </c>
@@ -17649,8 +17659,9 @@
       <c r="E300">
         <v>111.67500000000003</v>
       </c>
-    </row>
-    <row r="301" spans="1:5">
+      <c r="R300" s="12"/>
+    </row>
+    <row r="301" spans="1:18">
       <c r="A301" t="s">
         <v>6</v>
       </c>
@@ -17664,10 +17675,11 @@
         <v>22</v>
       </c>
       <c r="E301">
-        <v>117.83333333333333</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5">
+        <v>117.825</v>
+      </c>
+      <c r="R301" s="12"/>
+    </row>
+    <row r="302" spans="1:18">
       <c r="A302" t="s">
         <v>6</v>
       </c>
@@ -17681,10 +17693,11 @@
         <v>23</v>
       </c>
       <c r="E302">
-        <v>132.39166666666668</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5">
+        <v>132.40833333333333</v>
+      </c>
+      <c r="R302" s="12"/>
+    </row>
+    <row r="303" spans="1:18">
       <c r="A303" t="s">
         <v>6</v>
       </c>
@@ -17700,8 +17713,9 @@
       <c r="E303">
         <v>114.22500000000001</v>
       </c>
-    </row>
-    <row r="304" spans="1:5">
+      <c r="R303" s="12"/>
+    </row>
+    <row r="304" spans="1:18">
       <c r="A304" t="s">
         <v>6</v>
       </c>
@@ -17732,7 +17746,7 @@
         <v>26</v>
       </c>
       <c r="E305">
-        <v>120.49166666666666</v>
+        <v>120.55833333333334</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -17783,7 +17797,7 @@
         <v>17</v>
       </c>
       <c r="E308">
-        <v>118.64999999999998</v>
+        <v>118.66666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -23081,7 +23095,7 @@
         <v>8</v>
       </c>
       <c r="E296">
-        <v>124.51666666666667</v>
+        <v>124.53333333333335</v>
       </c>
     </row>
     <row r="297" spans="1:5">
@@ -23132,7 +23146,7 @@
         <v>20</v>
       </c>
       <c r="E299">
-        <v>90.016666666666666</v>
+        <v>90.024999999999991</v>
       </c>
     </row>
     <row r="300" spans="1:5">
@@ -23166,7 +23180,7 @@
         <v>22</v>
       </c>
       <c r="E301">
-        <v>114.05833333333332</v>
+        <v>114.04166666666667</v>
       </c>
     </row>
     <row r="302" spans="1:5">
@@ -23183,7 +23197,7 @@
         <v>23</v>
       </c>
       <c r="E302">
-        <v>130.30833333333337</v>
+        <v>130.31666666666669</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -23200,7 +23214,7 @@
         <v>24</v>
       </c>
       <c r="E303">
-        <v>123.06666666666668</v>
+        <v>123.11666666666667</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -23234,7 +23248,7 @@
         <v>26</v>
       </c>
       <c r="E305">
-        <v>108.3</v>
+        <v>108.45</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -23268,7 +23282,7 @@
         <v>28</v>
       </c>
       <c r="E307">
-        <v>141.93333333333331</v>
+        <v>141.94999999999999</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -23285,7 +23299,7 @@
         <v>17</v>
       </c>
       <c r="E308">
-        <v>119.13333333333333</v>
+        <v>119.14999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -23299,7 +23313,7 @@
   <dimension ref="B1:AF308"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z296" sqref="Z296:AF308"/>
     </sheetView>
   </sheetViews>
@@ -39961,7 +39975,7 @@
         <v>36</v>
       </c>
       <c r="F296">
-        <v>130.37500000000003</v>
+        <v>130.4</v>
       </c>
       <c r="G296" t="s">
         <v>37</v>
@@ -39979,7 +39993,7 @@
         <v>36</v>
       </c>
       <c r="N296">
-        <v>131.65833333333333</v>
+        <v>131.67499999999998</v>
       </c>
       <c r="O296" t="s">
         <v>37</v>
@@ -39997,7 +40011,7 @@
         <v>36</v>
       </c>
       <c r="V296">
-        <v>120.75833333333333</v>
+        <v>120.76666666666667</v>
       </c>
       <c r="W296" t="s">
         <v>37</v>
@@ -40015,7 +40029,7 @@
         <v>36</v>
       </c>
       <c r="AD296">
-        <v>124.51666666666667</v>
+        <v>124.53333333333335</v>
       </c>
       <c r="AE296" t="s">
         <v>37</v>
@@ -40029,7 +40043,7 @@
         <v>36</v>
       </c>
       <c r="F297">
-        <v>151.98333333333329</v>
+        <v>152.01666666666662</v>
       </c>
       <c r="G297" t="s">
         <v>37</v>
@@ -40041,7 +40055,7 @@
         <v>36</v>
       </c>
       <c r="N297">
-        <v>154.13333333333333</v>
+        <v>154.17499999999998</v>
       </c>
       <c r="O297" t="s">
         <v>37</v>
@@ -40053,7 +40067,7 @@
         <v>36</v>
       </c>
       <c r="V297">
-        <v>135.55833333333337</v>
+        <v>135.56666666666669</v>
       </c>
       <c r="W297" t="s">
         <v>37</v>
@@ -40079,7 +40093,7 @@
         <v>36</v>
       </c>
       <c r="F298">
-        <v>171.24166666666667</v>
+        <v>171.22499999999999</v>
       </c>
       <c r="G298" t="s">
         <v>37</v>
@@ -40091,7 +40105,7 @@
         <v>36</v>
       </c>
       <c r="N298">
-        <v>173.04166666666666</v>
+        <v>173.02499999999998</v>
       </c>
       <c r="O298" t="s">
         <v>37</v>
@@ -40103,7 +40117,7 @@
         <v>36</v>
       </c>
       <c r="V298">
-        <v>173.35833333333335</v>
+        <v>173.36666666666667</v>
       </c>
       <c r="W298" t="s">
         <v>37</v>
@@ -40153,7 +40167,7 @@
         <v>36</v>
       </c>
       <c r="V299">
-        <v>91.008333333333326</v>
+        <v>90.999999999999986</v>
       </c>
       <c r="W299" t="s">
         <v>37</v>
@@ -40165,7 +40179,7 @@
         <v>36</v>
       </c>
       <c r="AD299">
-        <v>90.016666666666666</v>
+        <v>90.024999999999991</v>
       </c>
       <c r="AE299" t="s">
         <v>37</v>
@@ -40253,7 +40267,7 @@
         <v>36</v>
       </c>
       <c r="V301">
-        <v>117.83333333333333</v>
+        <v>117.825</v>
       </c>
       <c r="W301" t="s">
         <v>37</v>
@@ -40265,7 +40279,7 @@
         <v>36</v>
       </c>
       <c r="AD301">
-        <v>114.05833333333332</v>
+        <v>114.04166666666667</v>
       </c>
       <c r="AE301" t="s">
         <v>37</v>
@@ -40279,7 +40293,7 @@
         <v>36</v>
       </c>
       <c r="F302">
-        <v>128.16666666666666</v>
+        <v>128.18333333333331</v>
       </c>
       <c r="G302" t="s">
         <v>37</v>
@@ -40291,7 +40305,7 @@
         <v>36</v>
       </c>
       <c r="N302">
-        <v>127.74166666666666</v>
+        <v>127.75833333333333</v>
       </c>
       <c r="O302" t="s">
         <v>37</v>
@@ -40303,7 +40317,7 @@
         <v>36</v>
       </c>
       <c r="V302">
-        <v>132.39166666666668</v>
+        <v>132.40833333333333</v>
       </c>
       <c r="W302" t="s">
         <v>37</v>
@@ -40315,7 +40329,7 @@
         <v>36</v>
       </c>
       <c r="AD302">
-        <v>130.30833333333337</v>
+        <v>130.31666666666669</v>
       </c>
       <c r="AE302" t="s">
         <v>37</v>
@@ -40329,7 +40343,7 @@
         <v>36</v>
       </c>
       <c r="F303">
-        <v>120.50000000000001</v>
+        <v>120.53333333333335</v>
       </c>
       <c r="G303" t="s">
         <v>37</v>
@@ -40341,7 +40355,7 @@
         <v>36</v>
       </c>
       <c r="N303">
-        <v>120.68333333333334</v>
+        <v>120.71666666666668</v>
       </c>
       <c r="O303" t="s">
         <v>37</v>
@@ -40365,7 +40379,7 @@
         <v>36</v>
       </c>
       <c r="AD303">
-        <v>123.06666666666668</v>
+        <v>123.11666666666667</v>
       </c>
       <c r="AE303" t="s">
         <v>37</v>
@@ -40379,7 +40393,7 @@
         <v>36</v>
       </c>
       <c r="F304">
-        <v>94.641666666666666</v>
+        <v>94.633333333333326</v>
       </c>
       <c r="G304" t="s">
         <v>37</v>
@@ -40391,7 +40405,7 @@
         <v>36</v>
       </c>
       <c r="N304">
-        <v>94.441666666666677</v>
+        <v>94.433333333333337</v>
       </c>
       <c r="O304" t="s">
         <v>37</v>
@@ -40429,7 +40443,7 @@
         <v>36</v>
       </c>
       <c r="F305">
-        <v>117.00833333333333</v>
+        <v>117.05</v>
       </c>
       <c r="G305" t="s">
         <v>37</v>
@@ -40441,7 +40455,7 @@
         <v>36</v>
       </c>
       <c r="N305">
-        <v>117.44166666666666</v>
+        <v>117.47500000000001</v>
       </c>
       <c r="O305" t="s">
         <v>37</v>
@@ -40453,7 +40467,7 @@
         <v>36</v>
       </c>
       <c r="V305">
-        <v>120.49166666666666</v>
+        <v>120.55833333333334</v>
       </c>
       <c r="W305" t="s">
         <v>37</v>
@@ -40465,7 +40479,7 @@
         <v>36</v>
       </c>
       <c r="AD305">
-        <v>108.3</v>
+        <v>108.45</v>
       </c>
       <c r="AE305" t="s">
         <v>37</v>
@@ -40529,7 +40543,7 @@
         <v>36</v>
       </c>
       <c r="F307">
-        <v>147.24999999999997</v>
+        <v>147.26666666666665</v>
       </c>
       <c r="G307" t="s">
         <v>37</v>
@@ -40541,7 +40555,7 @@
         <v>36</v>
       </c>
       <c r="N307">
-        <v>147.30833333333334</v>
+        <v>147.33333333333334</v>
       </c>
       <c r="O307" t="s">
         <v>37</v>
@@ -40565,7 +40579,7 @@
         <v>36</v>
       </c>
       <c r="AD307">
-        <v>141.93333333333331</v>
+        <v>141.94999999999999</v>
       </c>
       <c r="AE307" t="s">
         <v>37</v>
@@ -40579,7 +40593,7 @@
         <v>36</v>
       </c>
       <c r="F308">
-        <v>121.78333333333332</v>
+        <v>121.80833333333332</v>
       </c>
       <c r="G308" t="s">
         <v>37</v>
@@ -40594,7 +40608,7 @@
         <v>36</v>
       </c>
       <c r="N308">
-        <v>122.24166666666669</v>
+        <v>122.27500000000002</v>
       </c>
       <c r="O308" t="s">
         <v>37</v>
@@ -40609,7 +40623,7 @@
         <v>36</v>
       </c>
       <c r="V308">
-        <v>118.64999999999998</v>
+        <v>118.66666666666664</v>
       </c>
       <c r="W308" t="s">
         <v>37</v>
@@ -40624,7 +40638,7 @@
         <v>36</v>
       </c>
       <c r="AD308">
-        <v>119.13333333333333</v>
+        <v>119.14999999999999</v>
       </c>
       <c r="AE308" t="s">
         <v>37</v>

</xml_diff>